<commit_message>
$FL start 19/20 Quarterly Results
</commit_message>
<xml_diff>
--- a/$FL.xlsx
+++ b/$FL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2209274-113D-46A4-843B-666C52E41833}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AC89D7-DBE9-4A6B-B976-25816F1037C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{77D9C7A4-F0C3-486A-8AA0-E7E6A2714164}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="136">
   <si>
     <t>$FL</t>
   </si>
@@ -428,6 +428,12 @@
   </si>
   <si>
     <t>(Projected)</t>
+  </si>
+  <si>
+    <t>Model NI</t>
+  </si>
+  <si>
+    <t>FY17</t>
   </si>
 </sst>
 </file>
@@ -667,7 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -751,42 +757,6 @@
     <xf numFmtId="17" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -818,6 +788,44 @@
     <xf numFmtId="9" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1307,7 +1315,7 @@
   <dimension ref="A2:Q41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+      <selection activeCell="C31" sqref="C31:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1326,24 +1334,24 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
-      <c r="G5" s="51" t="s">
+      <c r="C5" s="72"/>
+      <c r="D5" s="73"/>
+      <c r="G5" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="53"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="73"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
@@ -1529,11 +1537,11 @@
       <c r="Q14" s="7"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="53"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="73"/>
       <c r="G15" s="15"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -1550,10 +1558,10 @@
       <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="48"/>
+      <c r="D16" s="69"/>
       <c r="G16" s="15"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1573,10 +1581,10 @@
       <c r="B17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="48"/>
+      <c r="D17" s="69"/>
       <c r="G17" s="15"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -1596,10 +1604,10 @@
       <c r="B18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="48"/>
+      <c r="D18" s="69"/>
       <c r="G18" s="15"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -1616,10 +1624,10 @@
       <c r="B19" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="50"/>
+      <c r="D19" s="77"/>
       <c r="G19" s="15"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -1659,11 +1667,11 @@
       <c r="Q21" s="7"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="53"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="73"/>
       <c r="G22" s="15"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -1680,10 +1688,10 @@
       <c r="B23" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="48"/>
+      <c r="D23" s="69"/>
       <c r="G23" s="15"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -1700,10 +1708,10 @@
       <c r="B24" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="47">
+      <c r="C24" s="68">
         <v>1879</v>
       </c>
-      <c r="D24" s="48"/>
+      <c r="D24" s="69"/>
       <c r="G24" s="15"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -1720,11 +1728,11 @@
       <c r="B25" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="58">
+      <c r="C25" s="70">
         <f>'Financial Model'!U33</f>
         <v>2794</v>
       </c>
-      <c r="D25" s="48"/>
+      <c r="D25" s="69"/>
       <c r="G25" s="15"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -1739,8 +1747,8 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B26" s="13"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="48"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="69"/>
       <c r="G26" s="15"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -1757,11 +1765,11 @@
       <c r="B27" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="58">
+      <c r="C27" s="70">
         <f>'Financial Model'!U33</f>
         <v>2794</v>
       </c>
-      <c r="D27" s="48"/>
+      <c r="D27" s="69"/>
       <c r="G27" s="15"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -1778,11 +1786,11 @@
       <c r="B28" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="58">
+      <c r="C28" s="70">
         <f>'Financial Model'!U42</f>
         <v>1685</v>
       </c>
-      <c r="D28" s="48"/>
+      <c r="D28" s="69"/>
       <c r="G28" s="15"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -1797,8 +1805,8 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B29" s="13"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="48"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="69"/>
       <c r="G29" s="15"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -1838,10 +1846,10 @@
       <c r="B31" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="54" t="s">
+      <c r="C31" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="55"/>
+      <c r="D31" s="75"/>
       <c r="G31" s="16"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
@@ -1855,83 +1863,81 @@
       <c r="Q31" s="9"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="51" t="s">
+      <c r="B34" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="52"/>
-      <c r="D34" s="53"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="73"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="56">
+      <c r="C35" s="66">
         <f>C6/'Financial Model'!U67</f>
         <v>1.1231500460263886</v>
       </c>
-      <c r="D35" s="57"/>
+      <c r="D35" s="67"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="56">
+      <c r="C36" s="66">
         <f>C8/SUM('Financial Model'!R6:U6)</f>
         <v>0.41777787687114459</v>
       </c>
-      <c r="D36" s="57"/>
+      <c r="D36" s="67"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="56">
+      <c r="C37" s="66">
         <f>C12/SUM('Financial Model'!R6:U6)</f>
         <v>0.42954392667694763</v>
       </c>
-      <c r="D37" s="57"/>
+      <c r="D37" s="67"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="56">
+      <c r="C38" s="66">
         <f>C6/SUM('Financial Model'!R18:U18)</f>
         <v>8.9160063090667094</v>
       </c>
-      <c r="D38" s="57"/>
+      <c r="D38" s="67"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="56">
+      <c r="C39" s="66">
         <f>C12/SUM('Financial Model'!R17:U17)</f>
         <v>8.8684611654009426</v>
       </c>
-      <c r="D39" s="57"/>
+      <c r="D39" s="67"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="47"/>
-      <c r="D40" s="48"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="69"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="14"/>
-      <c r="C41" s="49"/>
-      <c r="D41" s="50"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
     <mergeCell ref="G5:Q5"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C31:D31"/>
@@ -1944,11 +1950,13 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C31:D31" r:id="rId1" display="Link" xr:uid="{895B3114-FB4F-46F5-A7E6-2022E34FF531}"/>
@@ -1964,10 +1972,10 @@
   <dimension ref="A1:AT86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U75" sqref="R75:U75"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="H26:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1975,9 +1983,9 @@
     <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="21" width="9.140625" style="1"/>
-    <col min="22" max="22" width="9.140625" style="66"/>
+    <col min="22" max="22" width="9.140625" style="54"/>
     <col min="23" max="34" width="9.140625" style="1"/>
-    <col min="35" max="35" width="9.140625" style="66"/>
+    <col min="35" max="35" width="9.140625" style="54"/>
     <col min="36" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -2009,10 +2017,10 @@
       <c r="K1" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="23" t="s">
         <v>39</v>
       </c>
       <c r="N1" s="22" t="s">
@@ -2039,7 +2047,7 @@
       <c r="U1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="V1" s="64" t="s">
+      <c r="V1" s="52" t="s">
         <v>48</v>
       </c>
       <c r="W1" s="22" t="s">
@@ -2057,6 +2065,9 @@
       <c r="AA1" s="22" t="s">
         <v>50</v>
       </c>
+      <c r="AD1" s="22" t="s">
+        <v>135</v>
+      </c>
       <c r="AE1" s="22" t="s">
         <v>53</v>
       </c>
@@ -2069,7 +2080,7 @@
       <c r="AH1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AI1" s="64" t="s">
+      <c r="AI1" s="52" t="s">
         <v>57</v>
       </c>
       <c r="AJ1" s="22" t="s">
@@ -2108,6 +2119,18 @@
     </row>
     <row r="2" spans="1:46" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25"/>
+      <c r="H2" s="27">
+        <v>43680</v>
+      </c>
+      <c r="I2" s="27">
+        <v>43771</v>
+      </c>
+      <c r="L2" s="27">
+        <v>44044</v>
+      </c>
+      <c r="M2" s="27">
+        <v>44135</v>
+      </c>
       <c r="O2" s="27">
         <v>44317</v>
       </c>
@@ -2129,7 +2152,7 @@
       <c r="U2" s="27">
         <v>44863</v>
       </c>
-      <c r="V2" s="65" t="s">
+      <c r="V2" s="53" t="s">
         <v>133</v>
       </c>
       <c r="AG2" s="27">
@@ -2138,12 +2161,18 @@
       <c r="AH2" s="27">
         <v>44590</v>
       </c>
-      <c r="AI2" s="65" t="s">
+      <c r="AI2" s="53" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:46" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25"/>
+      <c r="L3" s="45">
+        <v>44409</v>
+      </c>
+      <c r="M3" s="45">
+        <v>44136</v>
+      </c>
       <c r="R3" s="45">
         <v>45689</v>
       </c>
@@ -2156,11 +2185,11 @@
       <c r="U3" s="45">
         <v>43405</v>
       </c>
-      <c r="V3" s="65"/>
+      <c r="V3" s="53"/>
       <c r="AH3" s="45">
         <v>45689</v>
       </c>
-      <c r="AI3" s="65"/>
+      <c r="AI3" s="53"/>
     </row>
     <row r="4" spans="1:46" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="39" t="s">
@@ -2171,12 +2200,20 @@
       <c r="E4" s="37"/>
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
+      <c r="H4" s="37">
+        <v>1521</v>
+      </c>
+      <c r="I4" s="37">
+        <v>1636</v>
+      </c>
       <c r="J4" s="37"/>
       <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
+      <c r="L4" s="37">
+        <v>1388</v>
+      </c>
+      <c r="M4" s="37">
+        <v>1656</v>
+      </c>
       <c r="N4" s="37"/>
       <c r="O4" s="37">
         <v>1620</v>
@@ -2200,7 +2237,7 @@
       <c r="U4" s="37">
         <v>1818</v>
       </c>
-      <c r="V4" s="66"/>
+      <c r="V4" s="54"/>
       <c r="AE4" s="37"/>
       <c r="AF4" s="37"/>
       <c r="AG4" s="37">
@@ -2209,7 +2246,7 @@
       <c r="AH4" s="37">
         <v>7029</v>
       </c>
-      <c r="AI4" s="66"/>
+      <c r="AI4" s="54"/>
     </row>
     <row r="5" spans="1:46" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="39" t="s">
@@ -2220,12 +2257,20 @@
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="H5" s="37">
+        <v>253</v>
+      </c>
+      <c r="I5" s="37">
+        <v>296</v>
+      </c>
       <c r="J5" s="37"/>
       <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
+      <c r="L5" s="37">
+        <v>689</v>
+      </c>
+      <c r="M5" s="37">
+        <v>450</v>
+      </c>
       <c r="N5" s="37"/>
       <c r="O5" s="37">
         <v>533</v>
@@ -2249,7 +2294,7 @@
       <c r="U5" s="37">
         <v>355</v>
       </c>
-      <c r="V5" s="66"/>
+      <c r="V5" s="54"/>
       <c r="AE5" s="37"/>
       <c r="AF5" s="37"/>
       <c r="AG5" s="37">
@@ -2258,7 +2303,7 @@
       <c r="AH5" s="37">
         <v>1929</v>
       </c>
-      <c r="AI5" s="66"/>
+      <c r="AI5" s="54"/>
     </row>
     <row r="6" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -2269,42 +2314,54 @@
       <c r="E6" s="34"/>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
+      <c r="H6" s="34">
+        <f t="shared" ref="H6:I6" si="0">H4+H5</f>
+        <v>1774</v>
+      </c>
+      <c r="I6" s="34">
+        <f t="shared" si="0"/>
+        <v>1932</v>
+      </c>
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
+      <c r="L6" s="34">
+        <f t="shared" ref="L6:U6" si="1">L4+L5</f>
+        <v>2077</v>
+      </c>
+      <c r="M6" s="34">
+        <f t="shared" si="1"/>
+        <v>2106</v>
+      </c>
       <c r="N6" s="34"/>
       <c r="O6" s="34">
-        <f>O4+O5</f>
+        <f t="shared" si="1"/>
         <v>2153</v>
       </c>
       <c r="P6" s="34">
-        <f>P4+P5</f>
+        <f t="shared" si="1"/>
         <v>2275</v>
       </c>
       <c r="Q6" s="34">
-        <f>Q4+Q5</f>
+        <f t="shared" si="1"/>
         <v>2189</v>
       </c>
       <c r="R6" s="34">
-        <f>R4+R5</f>
+        <f t="shared" si="1"/>
         <v>2341</v>
       </c>
       <c r="S6" s="34">
-        <f>S4+S5</f>
+        <f t="shared" si="1"/>
         <v>2175</v>
       </c>
       <c r="T6" s="34">
-        <f>T4+T5</f>
+        <f t="shared" si="1"/>
         <v>2065</v>
       </c>
       <c r="U6" s="34">
-        <f>U4+U5</f>
+        <f t="shared" si="1"/>
         <v>2173</v>
       </c>
-      <c r="V6" s="74">
+      <c r="V6" s="62">
         <f>U6*(1+V24)</f>
         <v>2281.65</v>
       </c>
@@ -2318,7 +2375,7 @@
         <f>AH4+AH5</f>
         <v>8958</v>
       </c>
-      <c r="AI6" s="74">
+      <c r="AI6" s="62">
         <f>SUM(S6:V6)</f>
         <v>8694.65</v>
       </c>
@@ -2332,12 +2389,20 @@
       <c r="E7" s="35"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
+      <c r="H7" s="35">
+        <v>1240</v>
+      </c>
+      <c r="I7" s="35">
+        <v>1312</v>
+      </c>
       <c r="J7" s="35"/>
       <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
+      <c r="L7" s="35">
+        <v>1539</v>
+      </c>
+      <c r="M7" s="35">
+        <v>1456</v>
+      </c>
       <c r="N7" s="35"/>
       <c r="O7" s="35">
         <v>1404</v>
@@ -2361,7 +2426,7 @@
       <c r="U7" s="35">
         <v>1477</v>
       </c>
-      <c r="V7" s="69">
+      <c r="V7" s="57">
         <f>V6*(1-V26)</f>
         <v>1551.5219999999999</v>
       </c>
@@ -2373,7 +2438,7 @@
       <c r="AH7" s="35">
         <v>5878</v>
       </c>
-      <c r="AI7" s="69">
+      <c r="AI7" s="57">
         <f>SUM(S7:V7)</f>
         <v>5874.5219999999999</v>
       </c>
@@ -2383,102 +2448,106 @@
         <v>78</v>
       </c>
       <c r="C8" s="34">
-        <f t="shared" ref="C8:T8" si="0">C6-C7</f>
+        <f t="shared" ref="C8:T8" si="2">C6-C7</f>
         <v>0</v>
       </c>
       <c r="D8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H8" s="34">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>534</v>
       </c>
       <c r="I8" s="34">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>620</v>
       </c>
       <c r="J8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L8" s="34">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>538</v>
       </c>
       <c r="M8" s="34">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>650</v>
       </c>
       <c r="N8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>749</v>
       </c>
       <c r="P8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>798</v>
       </c>
       <c r="Q8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>760</v>
       </c>
       <c r="R8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>773</v>
       </c>
       <c r="S8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>740</v>
       </c>
       <c r="T8" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>654</v>
       </c>
       <c r="U8" s="34">
         <f>U6-U7</f>
         <v>696</v>
       </c>
-      <c r="V8" s="74">
+      <c r="V8" s="62">
         <f>V6-V7</f>
         <v>730.12800000000016</v>
       </c>
+      <c r="AD8" s="34">
+        <f t="shared" ref="AD8:AE8" si="3">AD6-AD7</f>
+        <v>0</v>
+      </c>
       <c r="AE8" s="34">
-        <f t="shared" ref="AE8:AG8" si="1">AE6-AE7</f>
+        <f t="shared" ref="AE8:AG8" si="4">AE6-AE7</f>
         <v>0</v>
       </c>
       <c r="AF8" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG8" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2183</v>
       </c>
       <c r="AH8" s="34">
         <f>AH6-AH7</f>
         <v>3080</v>
       </c>
-      <c r="AI8" s="74">
+      <c r="AI8" s="62">
         <f>AI6-AI7</f>
         <v>2820.1279999999997</v>
       </c>
@@ -2492,12 +2561,20 @@
       <c r="E9" s="35"/>
       <c r="F9" s="35"/>
       <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
+      <c r="H9" s="35">
+        <v>393</v>
+      </c>
+      <c r="I9" s="35">
+        <v>411</v>
+      </c>
       <c r="J9" s="35"/>
       <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
+      <c r="L9" s="35">
+        <v>387</v>
+      </c>
+      <c r="M9" s="35">
+        <v>424</v>
+      </c>
       <c r="N9" s="35"/>
       <c r="O9" s="35">
         <v>418</v>
@@ -2509,7 +2586,7 @@
         <v>458</v>
       </c>
       <c r="R9" s="35">
-        <f t="shared" ref="R9:R11" si="2">AH9-SUM(O9:Q9)</f>
+        <f t="shared" ref="R9:R11" si="5">AH9-SUM(O9:Q9)</f>
         <v>525</v>
       </c>
       <c r="S9" s="35">
@@ -2521,7 +2598,7 @@
       <c r="U9" s="35">
         <v>467</v>
       </c>
-      <c r="V9" s="69">
+      <c r="V9" s="57">
         <f>V6*0.21</f>
         <v>479.1465</v>
       </c>
@@ -2529,6 +2606,7 @@
       <c r="Y9" s="30"/>
       <c r="Z9" s="30"/>
       <c r="AA9" s="30"/>
+      <c r="AD9" s="35"/>
       <c r="AE9" s="35"/>
       <c r="AF9" s="35"/>
       <c r="AG9" s="35">
@@ -2537,8 +2615,8 @@
       <c r="AH9" s="35">
         <v>1851</v>
       </c>
-      <c r="AI9" s="69">
-        <f t="shared" ref="AI9:AI11" si="3">SUM(S9:V9)</f>
+      <c r="AI9" s="57">
+        <f t="shared" ref="AI9:AI11" si="6">SUM(S9:V9)</f>
         <v>1861.1465000000001</v>
       </c>
     </row>
@@ -2551,12 +2629,20 @@
       <c r="E10" s="35"/>
       <c r="F10" s="35"/>
       <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
+      <c r="H10" s="35">
+        <v>46</v>
+      </c>
+      <c r="I10" s="35">
+        <v>44</v>
+      </c>
       <c r="J10" s="35"/>
       <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
+      <c r="L10" s="35">
+        <v>44</v>
+      </c>
+      <c r="M10" s="35">
+        <v>44</v>
+      </c>
       <c r="N10" s="35"/>
       <c r="O10" s="35">
         <v>45</v>
@@ -2568,7 +2654,7 @@
         <v>49</v>
       </c>
       <c r="R10" s="35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>55</v>
       </c>
       <c r="S10" s="35">
@@ -2580,10 +2666,11 @@
       <c r="U10" s="35">
         <v>52</v>
       </c>
-      <c r="V10" s="69">
+      <c r="V10" s="57">
         <f>AVERAGE(R10:U10)</f>
         <v>53</v>
       </c>
+      <c r="AD10" s="35"/>
       <c r="AE10" s="35"/>
       <c r="AF10" s="35"/>
       <c r="AG10" s="35">
@@ -2592,8 +2679,8 @@
       <c r="AH10" s="35">
         <v>197</v>
       </c>
-      <c r="AI10" s="69">
-        <f t="shared" si="3"/>
+      <c r="AI10" s="57">
+        <f t="shared" si="6"/>
         <v>210</v>
       </c>
     </row>
@@ -2606,12 +2693,20 @@
       <c r="E11" s="35"/>
       <c r="F11" s="35"/>
       <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
+      <c r="H11" s="35">
+        <v>14</v>
+      </c>
+      <c r="I11" s="35">
+        <v>1</v>
+      </c>
       <c r="J11" s="35"/>
       <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
+      <c r="L11" s="35">
+        <v>38</v>
+      </c>
+      <c r="M11" s="35">
+        <v>4</v>
+      </c>
       <c r="N11" s="35"/>
       <c r="O11" s="35">
         <v>4</v>
@@ -2623,7 +2718,7 @@
         <v>57</v>
       </c>
       <c r="R11" s="35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
       <c r="S11" s="35">
@@ -2635,10 +2730,11 @@
       <c r="U11" s="35">
         <v>20</v>
       </c>
-      <c r="V11" s="69">
+      <c r="V11" s="57">
         <f>AVERAGE(R11:U11)</f>
         <v>28.25</v>
       </c>
+      <c r="AD11" s="35"/>
       <c r="AE11" s="35"/>
       <c r="AF11" s="35"/>
       <c r="AG11" s="35">
@@ -2647,8 +2743,8 @@
       <c r="AH11" s="35">
         <v>172</v>
       </c>
-      <c r="AI11" s="69">
-        <f t="shared" si="3"/>
+      <c r="AI11" s="57">
+        <f t="shared" si="6"/>
         <v>66.25</v>
       </c>
     </row>
@@ -2657,103 +2753,107 @@
         <v>82</v>
       </c>
       <c r="C12" s="34">
-        <f t="shared" ref="C12:T12" si="4">C8-C9-C10-C11</f>
+        <f t="shared" ref="C12:T12" si="7">C8-C9-C10-C11</f>
         <v>0</v>
       </c>
       <c r="D12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H12" s="34">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>81</v>
       </c>
       <c r="I12" s="34">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>164</v>
       </c>
       <c r="J12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L12" s="34">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>69</v>
       </c>
       <c r="M12" s="34">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>178</v>
       </c>
       <c r="N12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>282</v>
       </c>
       <c r="P12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>264</v>
       </c>
       <c r="Q12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>196</v>
       </c>
       <c r="R12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>118</v>
       </c>
       <c r="S12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>217</v>
       </c>
       <c r="T12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>139</v>
       </c>
       <c r="U12" s="34">
         <f>U8-U9-U10-U11</f>
         <v>157</v>
       </c>
-      <c r="V12" s="74">
+      <c r="V12" s="62">
         <f>V8-V9-V10-V11</f>
         <v>169.73150000000015</v>
       </c>
+      <c r="AD12" s="34">
+        <f t="shared" ref="AD12:AE12" si="8">AD8-AD9-AD10-AD11</f>
+        <v>0</v>
+      </c>
       <c r="AE12" s="34">
-        <f t="shared" ref="AE12:AI12" si="5">AE8-AE9-AE10-AE11</f>
+        <f t="shared" ref="AE12:AI12" si="9">AE8-AE9-AE10-AE11</f>
         <v>0</v>
       </c>
       <c r="AF12" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG12" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>303</v>
       </c>
       <c r="AH12" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>860</v>
       </c>
-      <c r="AI12" s="74">
-        <f t="shared" si="5"/>
+      <c r="AI12" s="62">
+        <f t="shared" si="9"/>
         <v>682.73149999999964</v>
       </c>
     </row>
@@ -2766,12 +2866,20 @@
       <c r="E13" s="35"/>
       <c r="F13" s="35"/>
       <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
+      <c r="H13" s="35">
+        <v>2</v>
+      </c>
+      <c r="I13" s="35">
+        <v>3</v>
+      </c>
       <c r="J13" s="35"/>
       <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
+      <c r="L13" s="35">
+        <v>-2</v>
+      </c>
+      <c r="M13" s="35">
+        <v>-2</v>
+      </c>
       <c r="N13" s="35"/>
       <c r="O13" s="35">
         <v>-2</v>
@@ -2783,7 +2891,7 @@
         <v>-4</v>
       </c>
       <c r="R13" s="35">
-        <f t="shared" ref="R13:R14" si="6">AH13-SUM(O13:Q13)</f>
+        <f t="shared" ref="R13:R14" si="10">AH13-SUM(O13:Q13)</f>
         <v>-6</v>
       </c>
       <c r="S13" s="35">
@@ -2795,10 +2903,11 @@
       <c r="U13" s="35">
         <v>-3</v>
       </c>
-      <c r="V13" s="69">
+      <c r="V13" s="57">
         <f>AVERAGE(R13:U13)</f>
         <v>-4.75</v>
       </c>
+      <c r="AD13" s="35"/>
       <c r="AE13" s="35"/>
       <c r="AF13" s="35"/>
       <c r="AG13" s="35">
@@ -2807,8 +2916,8 @@
       <c r="AH13" s="35">
         <v>-14</v>
       </c>
-      <c r="AI13" s="69">
-        <f t="shared" ref="AI13:AI14" si="7">SUM(S13:V13)</f>
+      <c r="AI13" s="57">
+        <f t="shared" ref="AI13:AI14" si="11">SUM(S13:V13)</f>
         <v>-17.75</v>
       </c>
     </row>
@@ -2821,12 +2930,20 @@
       <c r="E14" s="35"/>
       <c r="F14" s="35"/>
       <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
+      <c r="H14" s="35">
+        <v>2</v>
+      </c>
+      <c r="I14" s="35">
+        <v>4</v>
+      </c>
       <c r="J14" s="35"/>
       <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
+      <c r="L14" s="35">
+        <v>3</v>
+      </c>
+      <c r="M14" s="35">
+        <v>193</v>
+      </c>
       <c r="N14" s="35"/>
       <c r="O14" s="35">
         <v>4</v>
@@ -2838,7 +2955,7 @@
         <v>30</v>
       </c>
       <c r="R14" s="35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>35</v>
       </c>
       <c r="S14" s="35">
@@ -2850,10 +2967,11 @@
       <c r="U14" s="35">
         <v>-11</v>
       </c>
-      <c r="V14" s="69">
+      <c r="V14" s="57">
         <f>AVERAGE(R14:U14)</f>
         <v>2.75</v>
       </c>
+      <c r="AD14" s="35"/>
       <c r="AE14" s="35"/>
       <c r="AF14" s="35"/>
       <c r="AG14" s="35">
@@ -2862,8 +2980,8 @@
       <c r="AH14" s="35">
         <v>394</v>
       </c>
-      <c r="AI14" s="69">
-        <f t="shared" si="7"/>
+      <c r="AI14" s="57">
+        <f t="shared" si="11"/>
         <v>-21.25</v>
       </c>
     </row>
@@ -2872,103 +2990,107 @@
         <v>85</v>
       </c>
       <c r="C15" s="35">
-        <f t="shared" ref="C15:T15" si="8">C12+C13+C14</f>
+        <f t="shared" ref="C15:T15" si="12">C12+C13+C14</f>
         <v>0</v>
       </c>
       <c r="D15" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E15" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F15" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G15" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H15" s="35">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>85</v>
       </c>
       <c r="I15" s="35">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>171</v>
       </c>
       <c r="J15" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K15" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L15" s="35">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>70</v>
       </c>
       <c r="M15" s="35">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>369</v>
       </c>
       <c r="N15" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O15" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>284</v>
       </c>
       <c r="P15" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>587</v>
       </c>
       <c r="Q15" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>222</v>
       </c>
       <c r="R15" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>147</v>
       </c>
       <c r="S15" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>190</v>
       </c>
       <c r="T15" s="35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>143</v>
       </c>
       <c r="U15" s="35">
         <f>U12+U13+U14</f>
         <v>143</v>
       </c>
-      <c r="V15" s="69">
+      <c r="V15" s="57">
         <f>V12+V13+V14</f>
         <v>167.73150000000015</v>
       </c>
+      <c r="AD15" s="35">
+        <f t="shared" ref="AD15:AE15" si="13">AD12+AD13+AD14</f>
+        <v>0</v>
+      </c>
       <c r="AE15" s="35">
-        <f t="shared" ref="AE15:AI15" si="9">AE12+AE13+AE14</f>
+        <f t="shared" ref="AE15:AI15" si="14">AE12+AE13+AE14</f>
         <v>0</v>
       </c>
       <c r="AF15" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AG15" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>494</v>
       </c>
       <c r="AH15" s="35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>1240</v>
       </c>
-      <c r="AI15" s="69">
-        <f t="shared" si="9"/>
+      <c r="AI15" s="57">
+        <f t="shared" si="14"/>
         <v>643.73149999999964</v>
       </c>
     </row>
@@ -2981,12 +3103,20 @@
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
       <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
+      <c r="H16" s="35">
+        <v>25</v>
+      </c>
+      <c r="I16" s="35">
+        <v>46</v>
+      </c>
       <c r="J16" s="35"/>
       <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
+      <c r="L16" s="35">
+        <v>25</v>
+      </c>
+      <c r="M16" s="35">
+        <v>104</v>
+      </c>
       <c r="N16" s="35"/>
       <c r="O16" s="35">
         <v>82</v>
@@ -3010,10 +3140,11 @@
       <c r="U16" s="35">
         <v>47</v>
       </c>
-      <c r="V16" s="69">
+      <c r="V16" s="57">
         <f>V15*V29</f>
         <v>55.351395000000053</v>
       </c>
+      <c r="AD16" s="35"/>
       <c r="AE16" s="35"/>
       <c r="AF16" s="35"/>
       <c r="AG16" s="35">
@@ -3022,7 +3153,7 @@
       <c r="AH16" s="35">
         <v>348</v>
       </c>
-      <c r="AI16" s="69">
+      <c r="AI16" s="57">
         <f>SUM(S16:V16)</f>
         <v>209.35139500000005</v>
       </c>
@@ -3032,103 +3163,108 @@
         <v>87</v>
       </c>
       <c r="C17" s="34">
-        <f t="shared" ref="C17:T17" si="10">C15-C16</f>
+        <f t="shared" ref="C17:T17" si="15">C15-C16</f>
         <v>0</v>
       </c>
       <c r="D17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="E17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="F17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="G17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H17" s="34">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>60</v>
       </c>
       <c r="I17" s="34">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>125</v>
       </c>
       <c r="J17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="K17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L17" s="34">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>45</v>
       </c>
       <c r="M17" s="34">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>265</v>
       </c>
       <c r="N17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>202</v>
       </c>
       <c r="P17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>430</v>
       </c>
       <c r="Q17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>158</v>
       </c>
       <c r="R17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>102</v>
       </c>
       <c r="S17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>132</v>
       </c>
       <c r="T17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>94</v>
       </c>
       <c r="U17" s="34">
         <f>U15-U16</f>
         <v>96</v>
       </c>
-      <c r="V17" s="74">
+      <c r="V17" s="62">
         <f>V15-V16</f>
         <v>112.3801050000001</v>
       </c>
+      <c r="W17" s="34"/>
+      <c r="AD17" s="34">
+        <f t="shared" ref="AD17:AE17" si="16">AD15-AD16</f>
+        <v>0</v>
+      </c>
       <c r="AE17" s="34">
-        <f t="shared" ref="AE17:AI17" si="11">AE15-AE16</f>
+        <f t="shared" ref="AE17:AI17" si="17">AE15-AE16</f>
         <v>0</v>
       </c>
       <c r="AF17" s="34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AG17" s="34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>323</v>
       </c>
       <c r="AH17" s="34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>892</v>
       </c>
-      <c r="AI17" s="74">
-        <f t="shared" si="11"/>
+      <c r="AI17" s="62">
+        <f t="shared" si="17"/>
         <v>434.38010499999962</v>
       </c>
     </row>
@@ -3141,74 +3277,86 @@
       <c r="E18" s="35"/>
       <c r="F18" s="35"/>
       <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
+      <c r="H18" s="28">
+        <f t="shared" ref="H18:I18" si="18">H17/H19</f>
+        <v>0.54151624548736466</v>
+      </c>
+      <c r="I18" s="28">
+        <f t="shared" si="18"/>
+        <v>1.1693171188026192</v>
+      </c>
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
+      <c r="L18" s="28">
+        <f t="shared" ref="L18:V18" si="19">L17/L19</f>
+        <v>0.43062200956937802</v>
+      </c>
+      <c r="M18" s="28">
+        <f t="shared" si="19"/>
+        <v>2.5383141762452106</v>
+      </c>
       <c r="N18" s="35"/>
       <c r="O18" s="28">
-        <f>O17/O19</f>
+        <f t="shared" si="19"/>
         <v>1.9498069498069499</v>
       </c>
       <c r="P18" s="28">
-        <f>P17/P19</f>
+        <f t="shared" si="19"/>
         <v>4.1425818882466281</v>
       </c>
       <c r="Q18" s="28">
-        <f>Q17/Q19</f>
+        <f t="shared" si="19"/>
         <v>1.5310077519379846</v>
       </c>
       <c r="R18" s="28">
-        <f>R17/R19</f>
+        <f t="shared" si="19"/>
         <v>0.99512195121951219</v>
       </c>
       <c r="S18" s="28">
-        <f>S17/S19</f>
+        <f t="shared" si="19"/>
         <v>1.3735691987513008</v>
       </c>
       <c r="T18" s="28">
-        <f>T17/T19</f>
+        <f t="shared" si="19"/>
         <v>0.99893730074388953</v>
       </c>
       <c r="U18" s="28">
-        <f>U17/U19</f>
+        <f t="shared" si="19"/>
         <v>1.0278372591006424</v>
       </c>
-      <c r="V18" s="76">
-        <f>V17/V19</f>
+      <c r="V18" s="64">
+        <f t="shared" si="19"/>
         <v>1.2032131156316928</v>
       </c>
       <c r="AG18" s="28">
-        <f t="shared" ref="AG18:AH18" si="12">AG17/AG19</f>
+        <f t="shared" ref="AG18:AH18" si="20">AG17/AG19</f>
         <v>3.0968360498561842</v>
       </c>
       <c r="AH18" s="28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>8.7024390243902445</v>
       </c>
-      <c r="AI18" s="77">
+      <c r="AI18" s="65">
         <f>AI17/AI19</f>
         <v>4.6507505888650922</v>
       </c>
     </row>
-    <row r="19" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
+    <row r="19" spans="2:35" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
+      <c r="H19" s="36">
+        <v>110.8</v>
+      </c>
+      <c r="I19" s="36">
+        <v>106.9</v>
+      </c>
+      <c r="L19" s="36">
+        <v>104.5</v>
+      </c>
+      <c r="M19" s="36">
+        <v>104.4</v>
+      </c>
       <c r="O19" s="36">
         <v>103.6</v>
       </c>
@@ -3231,17 +3379,17 @@
       <c r="U19" s="36">
         <v>93.4</v>
       </c>
-      <c r="V19" s="69">
+      <c r="V19" s="79">
         <f>U19</f>
         <v>93.4</v>
       </c>
-      <c r="AG19" s="1">
+      <c r="AG19" s="36">
         <v>104.3</v>
       </c>
-      <c r="AH19" s="1">
+      <c r="AH19" s="36">
         <v>102.5</v>
       </c>
-      <c r="AI19" s="69">
+      <c r="AI19" s="79">
         <f>V19</f>
         <v>93.4</v>
       </c>
@@ -3250,19 +3398,27 @@
       <c r="B21" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="L21" s="29">
+        <f t="shared" ref="L21" si="21">L6/H6-1</f>
+        <v>0.17080045095828633</v>
+      </c>
+      <c r="M21" s="29">
+        <f t="shared" ref="M21" si="22">M6/I6-1</f>
+        <v>9.0062111801242128E-2</v>
+      </c>
       <c r="S21" s="29">
-        <f t="shared" ref="S21" si="13">S6/O6-1</f>
+        <f t="shared" ref="S21" si="23">S6/O6-1</f>
         <v>1.021830004644686E-2</v>
       </c>
       <c r="T21" s="29">
-        <f t="shared" ref="T21" si="14">T6/P6-1</f>
+        <f t="shared" ref="T21" si="24">T6/P6-1</f>
         <v>-9.2307692307692313E-2</v>
       </c>
       <c r="U21" s="29">
         <f>U6/Q6-1</f>
         <v>-7.3092736409319237E-3</v>
       </c>
-      <c r="V21" s="75">
+      <c r="V21" s="63">
         <f>V6/R6-1</f>
         <v>-2.5352413498504922E-2</v>
       </c>
@@ -3270,61 +3426,85 @@
         <f>AH6/AG6-1</f>
         <v>0.18680445151033376</v>
       </c>
-      <c r="AI21" s="75">
+      <c r="AI21" s="63">
         <f>AI6/AH6-1</f>
         <v>-2.9398303192677E-2</v>
       </c>
     </row>
     <row r="22" spans="2:35" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="51" t="s">
         <v>125</v>
       </c>
+      <c r="L22" s="40">
+        <f t="shared" ref="L22:L23" si="25">L4/H4-1</f>
+        <v>-8.7442472057856713E-2</v>
+      </c>
+      <c r="M22" s="40">
+        <f t="shared" ref="M22:M23" si="26">M4/I4-1</f>
+        <v>1.2224938875305513E-2</v>
+      </c>
       <c r="S22" s="40">
-        <f t="shared" ref="S22:S23" si="15">S4/O4-1</f>
+        <f t="shared" ref="S22:S23" si="27">S4/O4-1</f>
         <v>9.6296296296296324E-2</v>
       </c>
       <c r="T22" s="40">
-        <f t="shared" ref="T22:T23" si="16">T4/P4-1</f>
+        <f t="shared" ref="T22:T23" si="28">T4/P4-1</f>
         <v>-5.5586130985140314E-2</v>
       </c>
       <c r="U22" s="40">
         <f>U4/Q4-1</f>
         <v>3.530751708428248E-2</v>
       </c>
-      <c r="V22" s="68"/>
+      <c r="V22" s="56"/>
       <c r="AH22" s="40">
         <f>AH4/AG4-1</f>
         <v>0.29043510189094923</v>
       </c>
-      <c r="AI22" s="68"/>
+      <c r="AI22" s="56"/>
     </row>
     <row r="23" spans="2:35" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="51" t="s">
         <v>126</v>
       </c>
+      <c r="L23" s="40">
+        <f t="shared" si="25"/>
+        <v>1.7233201581027666</v>
+      </c>
+      <c r="M23" s="40">
+        <f t="shared" si="26"/>
+        <v>0.52027027027027017</v>
+      </c>
       <c r="S23" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="27"/>
         <v>-0.25140712945590993</v>
       </c>
       <c r="T23" s="40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="28"/>
         <v>-0.23799126637554591</v>
       </c>
       <c r="U23" s="40">
         <f>U5/Q5-1</f>
         <v>-0.18013856812933027</v>
       </c>
-      <c r="V23" s="68"/>
+      <c r="V23" s="56"/>
       <c r="AH23" s="40">
         <f>AH5/AG5-1</f>
         <v>-8.186577820085672E-2</v>
       </c>
-      <c r="AI23" s="68"/>
+      <c r="AI23" s="56"/>
     </row>
     <row r="24" spans="2:35" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="30" t="s">
         <v>90</v>
       </c>
+      <c r="I24" s="30">
+        <f>I6/H6-1</f>
+        <v>8.9064261555806157E-2</v>
+      </c>
+      <c r="M24" s="30">
+        <f>M6/L6-1</f>
+        <v>1.3962445835339343E-2</v>
+      </c>
       <c r="P24" s="30">
         <f>P6/O6-1</f>
         <v>5.666511843938693E-2</v>
@@ -3334,48 +3514,64 @@
         <v>-3.7802197802197846E-2</v>
       </c>
       <c r="R24" s="30">
-        <f t="shared" ref="R24:T24" si="17">R6/Q6-1</f>
+        <f t="shared" ref="R24:T24" si="29">R6/Q6-1</f>
         <v>6.9438099588853275E-2</v>
       </c>
       <c r="S24" s="30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="29"/>
         <v>-7.0909867577958141E-2</v>
       </c>
       <c r="T24" s="30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="29"/>
         <v>-5.0574712643678188E-2</v>
       </c>
       <c r="U24" s="30">
         <f>U6/T6-1</f>
         <v>5.2300242130750574E-2</v>
       </c>
-      <c r="V24" s="68">
+      <c r="V24" s="56">
         <v>0.05</v>
       </c>
-      <c r="AE24" s="62" t="s">
+      <c r="AE24" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="AF24" s="62" t="s">
+      <c r="AF24" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="AG24" s="62" t="s">
+      <c r="AG24" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="AH24" s="62" t="s">
+      <c r="AH24" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="AI24" s="68"/>
+      <c r="AI24" s="56"/>
     </row>
     <row r="26" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="H26" s="30">
+        <f t="shared" ref="H26:I26" si="30">H8/H6</f>
+        <v>0.30101465614430667</v>
+      </c>
+      <c r="I26" s="30">
+        <f t="shared" si="30"/>
+        <v>0.32091097308488614</v>
+      </c>
+      <c r="L26" s="30">
+        <f t="shared" ref="L26:M26" si="31">L8/L6</f>
+        <v>0.2590274434280212</v>
+      </c>
+      <c r="M26" s="30">
+        <f t="shared" ref="M26:O26" si="32">M8/M6</f>
+        <v>0.30864197530864196</v>
+      </c>
       <c r="O26" s="30">
-        <f t="shared" ref="O26" si="18">O8/O6</f>
+        <f t="shared" si="32"/>
         <v>0.34788666976312121</v>
       </c>
       <c r="P26" s="30">
-        <f t="shared" ref="P26:Q26" si="19">P8/P6</f>
+        <f t="shared" ref="P26" si="33">P8/P6</f>
         <v>0.35076923076923078</v>
       </c>
       <c r="Q26" s="30">
@@ -3383,22 +3579,22 @@
         <v>0.34719049794426676</v>
       </c>
       <c r="R26" s="30">
-        <f t="shared" ref="R26:S26" si="20">R8/R6</f>
+        <f t="shared" ref="R26" si="34">R8/R6</f>
         <v>0.33020076890217853</v>
       </c>
       <c r="S26" s="30">
-        <f t="shared" ref="S26:T26" si="21">S8/S6</f>
+        <f t="shared" ref="S26" si="35">S8/S6</f>
         <v>0.34022988505747126</v>
       </c>
       <c r="T26" s="30">
-        <f t="shared" ref="T26:U26" si="22">T8/T6</f>
+        <f t="shared" ref="T26" si="36">T8/T6</f>
         <v>0.31670702179176757</v>
       </c>
       <c r="U26" s="30">
         <f>U8/U6</f>
         <v>0.32029452369995398</v>
       </c>
-      <c r="V26" s="68">
+      <c r="V26" s="56">
         <v>0.32</v>
       </c>
       <c r="AG26" s="30">
@@ -3409,7 +3605,7 @@
         <f>AH8/AH6</f>
         <v>0.34382674704175037</v>
       </c>
-      <c r="AI26" s="68">
+      <c r="AI26" s="56">
         <f>AI8/AI6</f>
         <v>0.32435210157970706</v>
       </c>
@@ -3418,12 +3614,28 @@
       <c r="B27" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="H27" s="30">
+        <f t="shared" ref="H27:I27" si="37">H12/H6</f>
+        <v>4.5659526493799327E-2</v>
+      </c>
+      <c r="I27" s="30">
+        <f t="shared" si="37"/>
+        <v>8.4886128364389232E-2</v>
+      </c>
+      <c r="L27" s="30">
+        <f t="shared" ref="L27:M27" si="38">L12/L6</f>
+        <v>3.3220991815117958E-2</v>
+      </c>
+      <c r="M27" s="30">
+        <f t="shared" ref="M27:O27" si="39">M12/M6</f>
+        <v>8.4520417853751181E-2</v>
+      </c>
       <c r="O27" s="30">
-        <f t="shared" ref="O27" si="23">O12/O6</f>
+        <f t="shared" si="39"/>
         <v>0.13098002786809104</v>
       </c>
       <c r="P27" s="30">
-        <f t="shared" ref="P27:Q27" si="24">P12/P6</f>
+        <f t="shared" ref="P27" si="40">P12/P6</f>
         <v>0.11604395604395605</v>
       </c>
       <c r="Q27" s="30">
@@ -3431,22 +3643,22 @@
         <v>8.9538602101416176E-2</v>
       </c>
       <c r="R27" s="30">
-        <f t="shared" ref="R27:S27" si="25">R12/R6</f>
+        <f t="shared" ref="R27" si="41">R12/R6</f>
         <v>5.0405809483126868E-2</v>
       </c>
       <c r="S27" s="30">
-        <f t="shared" ref="S27:T27" si="26">S12/S6</f>
+        <f t="shared" ref="S27" si="42">S12/S6</f>
         <v>9.9770114942528743E-2</v>
       </c>
       <c r="T27" s="30">
-        <f t="shared" ref="T27:U27" si="27">T12/T6</f>
+        <f t="shared" ref="T27" si="43">T12/T6</f>
         <v>6.7312348668280869E-2</v>
       </c>
       <c r="U27" s="30">
         <f>U12/U6</f>
         <v>7.2250345144960884E-2</v>
       </c>
-      <c r="V27" s="68">
+      <c r="V27" s="56">
         <f>V12/V6</f>
         <v>7.4389805623123681E-2</v>
       </c>
@@ -3458,7 +3670,7 @@
         <f>AH12/AH6</f>
         <v>9.6003572225943287E-2</v>
       </c>
-      <c r="AI27" s="68">
+      <c r="AI27" s="56">
         <f>AI12/AI6</f>
         <v>7.8523172295607027E-2</v>
       </c>
@@ -3467,12 +3679,28 @@
       <c r="B28" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="H28" s="30">
+        <f t="shared" ref="H28:I28" si="44">H17/H6</f>
+        <v>3.3821871476888386E-2</v>
+      </c>
+      <c r="I28" s="30">
+        <f t="shared" si="44"/>
+        <v>6.4699792960662528E-2</v>
+      </c>
+      <c r="L28" s="30">
+        <f t="shared" ref="L28:M28" si="45">L17/L6</f>
+        <v>2.1665864227250843E-2</v>
+      </c>
+      <c r="M28" s="30">
+        <f t="shared" ref="M28:O28" si="46">M17/M6</f>
+        <v>0.12583095916429249</v>
+      </c>
       <c r="O28" s="30">
-        <f t="shared" ref="O28" si="28">O17/O6</f>
+        <f t="shared" si="46"/>
         <v>9.3822573153738972E-2</v>
       </c>
       <c r="P28" s="30">
-        <f t="shared" ref="P28:Q28" si="29">P17/P6</f>
+        <f t="shared" ref="P28" si="47">P17/P6</f>
         <v>0.18901098901098901</v>
       </c>
       <c r="Q28" s="30">
@@ -3480,22 +3708,22 @@
         <v>7.2179077204202829E-2</v>
       </c>
       <c r="R28" s="30">
-        <f t="shared" ref="R28:S28" si="30">R17/R6</f>
+        <f t="shared" ref="R28" si="48">R17/R6</f>
         <v>4.3571123451516446E-2</v>
       </c>
       <c r="S28" s="30">
-        <f t="shared" ref="S28:T28" si="31">S17/S6</f>
+        <f t="shared" ref="S28" si="49">S17/S6</f>
         <v>6.0689655172413794E-2</v>
       </c>
       <c r="T28" s="30">
-        <f t="shared" ref="T28:U28" si="32">T17/T6</f>
+        <f t="shared" ref="T28" si="50">T17/T6</f>
         <v>4.5520581113801452E-2</v>
       </c>
       <c r="U28" s="30">
         <f>U17/U6</f>
         <v>4.4178554993097099E-2</v>
       </c>
-      <c r="V28" s="68">
+      <c r="V28" s="56">
         <f>V17/V6</f>
         <v>4.9253875484846533E-2</v>
       </c>
@@ -3507,7 +3735,7 @@
         <f>AH17/AH6</f>
         <v>9.9575798169234203E-2</v>
       </c>
-      <c r="AI28" s="68">
+      <c r="AI28" s="56">
         <f>AI17/AI6</f>
         <v>4.9959469903906387E-2</v>
       </c>
@@ -3516,12 +3744,28 @@
       <c r="B29" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="H29" s="30">
+        <f t="shared" ref="H29:I29" si="51">H16/H15</f>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="I29" s="30">
+        <f t="shared" si="51"/>
+        <v>0.26900584795321636</v>
+      </c>
+      <c r="L29" s="30">
+        <f t="shared" ref="L29:M29" si="52">L16/L15</f>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="M29" s="30">
+        <f t="shared" ref="M29:O29" si="53">M16/M15</f>
+        <v>0.28184281842818426</v>
+      </c>
       <c r="O29" s="30">
-        <f t="shared" ref="O29" si="33">O16/O15</f>
+        <f t="shared" si="53"/>
         <v>0.28873239436619719</v>
       </c>
       <c r="P29" s="30">
-        <f t="shared" ref="P29:Q29" si="34">P16/P15</f>
+        <f t="shared" ref="P29" si="54">P16/P15</f>
         <v>0.26746166950596251</v>
       </c>
       <c r="Q29" s="30">
@@ -3529,22 +3773,22 @@
         <v>0.28828828828828829</v>
       </c>
       <c r="R29" s="30">
-        <f t="shared" ref="R29:S29" si="35">R16/R15</f>
+        <f t="shared" ref="R29" si="55">R16/R15</f>
         <v>0.30612244897959184</v>
       </c>
       <c r="S29" s="30">
-        <f t="shared" ref="S29:T29" si="36">S16/S15</f>
+        <f t="shared" ref="S29" si="56">S16/S15</f>
         <v>0.30526315789473685</v>
       </c>
       <c r="T29" s="30">
-        <f t="shared" ref="T29:U29" si="37">T16/T15</f>
+        <f t="shared" ref="T29" si="57">T16/T15</f>
         <v>0.34265734265734266</v>
       </c>
       <c r="U29" s="30">
         <f>U16/U15</f>
         <v>0.32867132867132864</v>
       </c>
-      <c r="V29" s="68">
+      <c r="V29" s="56">
         <v>0.33</v>
       </c>
       <c r="AG29" s="30">
@@ -3555,7 +3799,7 @@
         <f>AH16/AH15</f>
         <v>0.28064516129032258</v>
       </c>
-      <c r="AI29" s="68">
+      <c r="AI29" s="56">
         <f>AI16/AI15</f>
         <v>0.32521539648129721</v>
       </c>
@@ -3565,8 +3809,22 @@
       <c r="U30" s="30"/>
     </row>
     <row r="31" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="Q31" s="30"/>
-      <c r="U31" s="30"/>
+      <c r="B31" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I31" s="78"/>
+      <c r="J31" s="78"/>
+      <c r="K31" s="78"/>
+      <c r="L31" s="78"/>
+      <c r="M31" s="78"/>
+      <c r="N31" s="78"/>
+      <c r="O31" s="78"/>
+      <c r="P31" s="78"/>
+      <c r="Q31" s="78"/>
+      <c r="R31" s="78"/>
+      <c r="S31" s="78"/>
+      <c r="T31" s="78"/>
+      <c r="U31" s="78"/>
     </row>
     <row r="32" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B32" s="31" t="s">
@@ -3579,6 +3837,12 @@
       <c r="B33" s="35" t="s">
         <v>128</v>
       </c>
+      <c r="I33" s="35">
+        <v>3160</v>
+      </c>
+      <c r="M33" s="35">
+        <v>3032</v>
+      </c>
       <c r="O33" s="35">
         <v>2952</v>
       </c>
@@ -3600,114 +3864,126 @@
       <c r="U33" s="35">
         <v>2794</v>
       </c>
-      <c r="V33" s="69"/>
+      <c r="V33" s="57"/>
       <c r="AG33" s="35">
         <v>2998</v>
       </c>
       <c r="AH33" s="35">
         <v>2858</v>
       </c>
-      <c r="AI33" s="69"/>
-    </row>
-    <row r="34" spans="2:35" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="59" t="s">
+      <c r="AI33" s="57"/>
+    </row>
+    <row r="34" spans="2:35" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="S34" s="60">
+      <c r="M34" s="48">
+        <f>M33-I33</f>
+        <v>-128</v>
+      </c>
+      <c r="S34" s="48">
         <f>S33-O33</f>
         <v>-137</v>
       </c>
-      <c r="T34" s="60">
+      <c r="T34" s="48">
         <f>T33-P33</f>
         <v>-112</v>
       </c>
-      <c r="U34" s="60">
+      <c r="U34" s="48">
         <f>U33-Q33</f>
         <v>-162</v>
       </c>
-      <c r="V34" s="70"/>
-      <c r="AH34" s="60">
+      <c r="V34" s="58"/>
+      <c r="AH34" s="48">
         <f>AH33-AG33</f>
         <v>-140</v>
       </c>
-      <c r="AI34" s="70"/>
+      <c r="AI34" s="58"/>
     </row>
     <row r="35" spans="2:35" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B35" s="41" t="s">
         <v>131</v>
       </c>
       <c r="P35" s="42">
-        <f t="shared" ref="P35:U35" si="38">P33-O33</f>
+        <f t="shared" ref="P35:T35" si="58">P33-O33</f>
         <v>-41</v>
       </c>
       <c r="Q35" s="42">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>45</v>
       </c>
       <c r="R35" s="42">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>-98</v>
       </c>
       <c r="S35" s="42">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>-43</v>
       </c>
       <c r="T35" s="42">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>-16</v>
       </c>
       <c r="U35" s="42">
         <f>U33-T33</f>
         <v>-5</v>
       </c>
-      <c r="V35" s="71"/>
-      <c r="AE35" s="61" t="s">
+      <c r="V35" s="59"/>
+      <c r="AE35" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="AF35" s="61" t="s">
+      <c r="AF35" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="AG35" s="61" t="s">
+      <c r="AG35" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="AH35" s="61" t="s">
+      <c r="AH35" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="AI35" s="71"/>
+      <c r="AI35" s="59"/>
     </row>
     <row r="36" spans="2:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B36" s="43" t="s">
         <v>130</v>
       </c>
+      <c r="I36" s="44">
+        <f t="shared" ref="I36" si="59">I4/I33</f>
+        <v>0.51772151898734176</v>
+      </c>
+      <c r="M36" s="44">
+        <f t="shared" ref="M36:U36" si="60">M4/M33</f>
+        <v>0.54617414248021112</v>
+      </c>
       <c r="O36" s="44">
-        <f>O4/O33</f>
+        <f t="shared" si="60"/>
         <v>0.54878048780487809</v>
       </c>
       <c r="P36" s="44">
-        <f>P4/P33</f>
+        <f t="shared" si="60"/>
         <v>0.62418412916523536</v>
       </c>
       <c r="Q36" s="44">
-        <f>Q4/Q33</f>
+        <f t="shared" si="60"/>
         <v>0.59404600811907982</v>
       </c>
       <c r="R36" s="44">
-        <f>R4/R33</f>
+        <f t="shared" si="60"/>
         <v>0.64240727781665496</v>
       </c>
       <c r="S36" s="44">
-        <f>S4/S33</f>
+        <f t="shared" si="60"/>
         <v>0.63090586145648309</v>
       </c>
       <c r="T36" s="44">
-        <f>T4/T33</f>
+        <f t="shared" si="60"/>
         <v>0.61307609860664525</v>
       </c>
       <c r="U36" s="44">
-        <f>U4/U33</f>
+        <f t="shared" si="60"/>
         <v>0.65068002863278451</v>
       </c>
-      <c r="V36" s="72"/>
+      <c r="V36" s="60"/>
       <c r="AG36" s="44">
         <f>AG4/AG33</f>
         <v>1.8168779186124082</v>
@@ -3716,12 +3992,12 @@
         <f>AH4/AH33</f>
         <v>2.459412176347096</v>
       </c>
-      <c r="AI36" s="72"/>
+      <c r="AI36" s="60"/>
     </row>
     <row r="37" spans="2:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B37" s="43"/>
-      <c r="V37" s="72"/>
-      <c r="AI37" s="72"/>
+      <c r="V37" s="60"/>
+      <c r="AI37" s="60"/>
     </row>
     <row r="40" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B40" s="31" t="s">
@@ -3738,11 +4014,15 @@
       <c r="F41" s="34"/>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
-      <c r="I41" s="34"/>
+      <c r="I41" s="34">
+        <v>744</v>
+      </c>
       <c r="J41" s="34"/>
       <c r="K41" s="34"/>
       <c r="L41" s="34"/>
-      <c r="M41" s="34"/>
+      <c r="M41" s="34">
+        <v>1393</v>
+      </c>
       <c r="N41" s="34"/>
       <c r="O41" s="34">
         <v>1963</v>
@@ -3765,8 +4045,8 @@
       <c r="U41" s="34">
         <v>351</v>
       </c>
-      <c r="V41" s="67"/>
-      <c r="AI41" s="67"/>
+      <c r="V41" s="55"/>
+      <c r="AI41" s="55"/>
     </row>
     <row r="42" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
@@ -3778,11 +4058,15 @@
       <c r="F42" s="34"/>
       <c r="G42" s="34"/>
       <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
+      <c r="I42" s="34">
+        <v>1304</v>
+      </c>
       <c r="J42" s="34"/>
       <c r="K42" s="34"/>
       <c r="L42" s="34"/>
-      <c r="M42" s="34"/>
+      <c r="M42" s="34">
+        <v>1193</v>
+      </c>
       <c r="N42" s="34"/>
       <c r="O42" s="34">
         <v>1021</v>
@@ -3805,8 +4089,8 @@
       <c r="U42" s="34">
         <v>1685</v>
       </c>
-      <c r="V42" s="67"/>
-      <c r="AI42" s="67"/>
+      <c r="V42" s="55"/>
+      <c r="AI42" s="55"/>
     </row>
     <row r="43" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
@@ -3818,11 +4102,15 @@
       <c r="F43" s="35"/>
       <c r="G43" s="35"/>
       <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
+      <c r="I43" s="35">
+        <v>299</v>
+      </c>
       <c r="J43" s="35"/>
       <c r="K43" s="35"/>
       <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
+      <c r="M43" s="35">
+        <v>237</v>
+      </c>
       <c r="N43" s="35"/>
       <c r="O43" s="35">
         <v>283</v>
@@ -3851,63 +4139,63 @@
         <v>98</v>
       </c>
       <c r="C44" s="35">
-        <f t="shared" ref="C44:T44" si="39">SUM(C41:C43)</f>
+        <f t="shared" ref="C44:T44" si="61">SUM(C41:C43)</f>
         <v>0</v>
       </c>
       <c r="D44" s="35">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="E44" s="35">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="F44" s="35">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="G44" s="35">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="H44" s="35">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="I44" s="35">
-        <f t="shared" si="39"/>
-        <v>0</v>
+        <f t="shared" si="61"/>
+        <v>2347</v>
       </c>
       <c r="J44" s="35">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="K44" s="35">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="L44" s="35">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="M44" s="35">
-        <f t="shared" si="39"/>
-        <v>0</v>
+        <f t="shared" si="61"/>
+        <v>2823</v>
       </c>
       <c r="N44" s="35">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="O44" s="35">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>3267</v>
       </c>
       <c r="P44" s="35">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>3178</v>
       </c>
       <c r="Q44" s="35">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>2893</v>
       </c>
       <c r="R44" s="35">
@@ -3915,11 +4203,11 @@
         <v>2363</v>
       </c>
       <c r="S44" s="35">
-        <f t="shared" ref="S44" si="40">SUM(S41:S43)</f>
+        <f t="shared" ref="S44" si="62">SUM(S41:S43)</f>
         <v>2233</v>
       </c>
       <c r="T44" s="35">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>2315</v>
       </c>
       <c r="U44" s="35">
@@ -3937,11 +4225,15 @@
       <c r="F45" s="35"/>
       <c r="G45" s="35"/>
       <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
+      <c r="I45" s="35">
+        <v>814</v>
+      </c>
       <c r="J45" s="35"/>
       <c r="K45" s="35"/>
       <c r="L45" s="35"/>
-      <c r="M45" s="35"/>
+      <c r="M45" s="35">
+        <v>773</v>
+      </c>
       <c r="N45" s="35"/>
       <c r="O45" s="35">
         <v>769</v>
@@ -3975,11 +4267,15 @@
       <c r="F46" s="35"/>
       <c r="G46" s="35"/>
       <c r="H46" s="35"/>
-      <c r="I46" s="35"/>
+      <c r="I46" s="35">
+        <v>2956</v>
+      </c>
       <c r="J46" s="35"/>
       <c r="K46" s="35"/>
       <c r="L46" s="35"/>
-      <c r="M46" s="35"/>
+      <c r="M46" s="35">
+        <v>2752</v>
+      </c>
       <c r="N46" s="35"/>
       <c r="O46" s="35">
         <v>2700</v>
@@ -4013,11 +4309,15 @@
       <c r="F47" s="35"/>
       <c r="G47" s="35"/>
       <c r="H47" s="35"/>
-      <c r="I47" s="35"/>
+      <c r="I47" s="35">
+        <v>93</v>
+      </c>
       <c r="J47" s="35"/>
       <c r="K47" s="35"/>
       <c r="L47" s="35"/>
-      <c r="M47" s="35"/>
+      <c r="M47" s="35">
+        <v>69</v>
+      </c>
       <c r="N47" s="35"/>
       <c r="O47" s="35">
         <v>101</v>
@@ -4051,11 +4351,17 @@
       <c r="F48" s="35"/>
       <c r="G48" s="35"/>
       <c r="H48" s="35"/>
-      <c r="I48" s="35"/>
+      <c r="I48" s="35">
+        <f>156+21</f>
+        <v>177</v>
+      </c>
       <c r="J48" s="35"/>
       <c r="K48" s="35"/>
       <c r="L48" s="35"/>
-      <c r="M48" s="35"/>
+      <c r="M48" s="35">
+        <f>158+18</f>
+        <v>176</v>
+      </c>
       <c r="N48" s="35"/>
       <c r="O48" s="35">
         <f>159+16</f>
@@ -4096,11 +4402,15 @@
       <c r="F49" s="35"/>
       <c r="G49" s="35"/>
       <c r="H49" s="35"/>
-      <c r="I49" s="35"/>
+      <c r="I49" s="35">
+        <v>151</v>
+      </c>
       <c r="J49" s="35"/>
       <c r="K49" s="35"/>
       <c r="L49" s="35"/>
-      <c r="M49" s="35"/>
+      <c r="M49" s="35">
+        <v>340</v>
+      </c>
       <c r="N49" s="35"/>
       <c r="O49" s="35">
         <v>342</v>
@@ -4134,11 +4444,15 @@
       <c r="F50" s="35"/>
       <c r="G50" s="35"/>
       <c r="H50" s="35"/>
-      <c r="I50" s="35"/>
+      <c r="I50" s="35">
+        <v>83</v>
+      </c>
       <c r="J50" s="35"/>
       <c r="K50" s="35"/>
       <c r="L50" s="35"/>
-      <c r="M50" s="35"/>
+      <c r="M50" s="35">
+        <v>85</v>
+      </c>
       <c r="N50" s="35"/>
       <c r="O50" s="35">
         <v>88</v>
@@ -4167,63 +4481,63 @@
         <v>105</v>
       </c>
       <c r="C51" s="35">
-        <f t="shared" ref="C51:T51" si="41">SUM(C45:C50)+C44</f>
+        <f t="shared" ref="C51:T51" si="63">SUM(C45:C50)+C44</f>
         <v>0</v>
       </c>
       <c r="D51" s="35">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="E51" s="35">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="F51" s="35">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="G51" s="35">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="H51" s="35">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="I51" s="35">
-        <f t="shared" si="41"/>
-        <v>0</v>
+        <f t="shared" si="63"/>
+        <v>6621</v>
       </c>
       <c r="J51" s="35">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="K51" s="35">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="L51" s="35">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="M51" s="35">
-        <f t="shared" si="41"/>
-        <v>0</v>
+        <f t="shared" si="63"/>
+        <v>7018</v>
       </c>
       <c r="N51" s="35">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="O51" s="35">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>7442</v>
       </c>
       <c r="P51" s="35">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>7585</v>
       </c>
       <c r="Q51" s="35">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>8211</v>
       </c>
       <c r="R51" s="35">
@@ -4231,11 +4545,11 @@
         <v>8135</v>
       </c>
       <c r="S51" s="35">
-        <f t="shared" ref="S51" si="42">SUM(S45:S50)+S44</f>
+        <f t="shared" ref="S51" si="64">SUM(S45:S50)+S44</f>
         <v>7878</v>
       </c>
       <c r="T51" s="35">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>7868</v>
       </c>
       <c r="U51" s="35">
@@ -4253,11 +4567,15 @@
       <c r="F53" s="35"/>
       <c r="G53" s="35"/>
       <c r="H53" s="35"/>
-      <c r="I53" s="35"/>
+      <c r="I53" s="35">
+        <v>396</v>
+      </c>
       <c r="J53" s="35"/>
       <c r="K53" s="35"/>
       <c r="L53" s="35"/>
-      <c r="M53" s="35"/>
+      <c r="M53" s="35">
+        <v>514</v>
+      </c>
       <c r="N53" s="35"/>
       <c r="O53" s="35">
         <v>658</v>
@@ -4291,11 +4609,15 @@
       <c r="F54" s="35"/>
       <c r="G54" s="35"/>
       <c r="H54" s="35"/>
-      <c r="I54" s="35"/>
+      <c r="I54" s="35">
+        <v>333</v>
+      </c>
       <c r="J54" s="35"/>
       <c r="K54" s="35"/>
       <c r="L54" s="35"/>
-      <c r="M54" s="35"/>
+      <c r="M54" s="35">
+        <v>451</v>
+      </c>
       <c r="N54" s="35"/>
       <c r="O54" s="35">
         <v>572</v>
@@ -4329,11 +4651,15 @@
       <c r="F55" s="34"/>
       <c r="G55" s="34"/>
       <c r="H55" s="34"/>
-      <c r="I55" s="34"/>
+      <c r="I55" s="34">
+        <v>0</v>
+      </c>
       <c r="J55" s="34"/>
       <c r="K55" s="34"/>
       <c r="L55" s="34"/>
-      <c r="M55" s="34"/>
+      <c r="M55" s="34">
+        <v>2</v>
+      </c>
       <c r="N55" s="34"/>
       <c r="O55" s="34">
         <v>101</v>
@@ -4356,8 +4682,8 @@
       <c r="U55" s="34">
         <v>6</v>
       </c>
-      <c r="V55" s="67"/>
-      <c r="AI55" s="67"/>
+      <c r="V55" s="55"/>
+      <c r="AI55" s="55"/>
     </row>
     <row r="56" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
@@ -4369,11 +4695,15 @@
       <c r="F56" s="35"/>
       <c r="G56" s="35"/>
       <c r="H56" s="35"/>
-      <c r="I56" s="35"/>
+      <c r="I56" s="35">
+        <v>508</v>
+      </c>
       <c r="J56" s="35"/>
       <c r="K56" s="35"/>
       <c r="L56" s="35"/>
-      <c r="M56" s="35"/>
+      <c r="M56" s="35">
+        <v>575</v>
+      </c>
       <c r="N56" s="35"/>
       <c r="O56" s="35">
         <v>582</v>
@@ -4402,63 +4732,63 @@
         <v>110</v>
       </c>
       <c r="C57" s="35">
-        <f t="shared" ref="C57:T57" si="43">SUM(C53:C56)</f>
+        <f t="shared" ref="C57:T57" si="65">SUM(C53:C56)</f>
         <v>0</v>
       </c>
       <c r="D57" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="E57" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="F57" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="G57" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="H57" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="I57" s="35">
-        <f t="shared" si="43"/>
-        <v>0</v>
+        <f t="shared" si="65"/>
+        <v>1237</v>
       </c>
       <c r="J57" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="K57" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="L57" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="M57" s="35">
-        <f t="shared" si="43"/>
-        <v>0</v>
+        <f t="shared" si="65"/>
+        <v>1542</v>
       </c>
       <c r="N57" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="O57" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>1913</v>
       </c>
       <c r="P57" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>1681</v>
       </c>
       <c r="Q57" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>1757</v>
       </c>
       <c r="R57" s="35">
@@ -4466,11 +4796,11 @@
         <v>1735</v>
       </c>
       <c r="S57" s="35">
-        <f t="shared" ref="S57" si="44">SUM(S53:S56)</f>
+        <f t="shared" ref="S57" si="66">SUM(S53:S56)</f>
         <v>1556</v>
       </c>
       <c r="T57" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="65"/>
         <v>1585</v>
       </c>
       <c r="U57" s="35">
@@ -4488,11 +4818,15 @@
       <c r="F58" s="34"/>
       <c r="G58" s="34"/>
       <c r="H58" s="34"/>
-      <c r="I58" s="34"/>
+      <c r="I58" s="34">
+        <v>122</v>
+      </c>
       <c r="J58" s="34"/>
       <c r="K58" s="34"/>
       <c r="L58" s="34"/>
-      <c r="M58" s="34"/>
+      <c r="M58" s="34">
+        <v>129</v>
+      </c>
       <c r="N58" s="34"/>
       <c r="O58" s="34">
         <v>8</v>
@@ -4515,8 +4849,8 @@
       <c r="U58" s="34">
         <v>448</v>
       </c>
-      <c r="V58" s="67"/>
-      <c r="AI58" s="67"/>
+      <c r="V58" s="55"/>
+      <c r="AI58" s="55"/>
     </row>
     <row r="59" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
@@ -4528,11 +4862,15 @@
       <c r="F59" s="35"/>
       <c r="G59" s="35"/>
       <c r="H59" s="35"/>
-      <c r="I59" s="35"/>
+      <c r="I59" s="35">
+        <v>2179</v>
+      </c>
       <c r="J59" s="35"/>
       <c r="K59" s="35"/>
       <c r="L59" s="35"/>
-      <c r="M59" s="35"/>
+      <c r="M59" s="35">
+        <v>2514</v>
+      </c>
       <c r="N59" s="35"/>
       <c r="O59" s="35">
         <v>2470</v>
@@ -4566,11 +4904,15 @@
       <c r="F60" s="35"/>
       <c r="G60" s="35"/>
       <c r="H60" s="35"/>
-      <c r="I60" s="35"/>
+      <c r="I60" s="35">
+        <v>116</v>
+      </c>
       <c r="J60" s="35"/>
       <c r="K60" s="35"/>
       <c r="L60" s="35"/>
-      <c r="M60" s="35"/>
+      <c r="M60" s="35">
+        <v>181</v>
+      </c>
       <c r="N60" s="35"/>
       <c r="O60" s="35">
         <v>121</v>
@@ -4599,63 +4941,63 @@
         <v>114</v>
       </c>
       <c r="C61" s="35">
-        <f t="shared" ref="C61:T61" si="45">SUM(C58:C60)+C57</f>
+        <f t="shared" ref="C61:T61" si="67">SUM(C58:C60)+C57</f>
         <v>0</v>
       </c>
       <c r="D61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="E61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="F61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="G61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="H61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="I61" s="35">
-        <f t="shared" si="45"/>
-        <v>0</v>
+        <f t="shared" si="67"/>
+        <v>3654</v>
       </c>
       <c r="J61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="K61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="L61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="M61" s="35">
-        <f t="shared" si="45"/>
-        <v>0</v>
+        <f t="shared" si="67"/>
+        <v>4366</v>
       </c>
       <c r="N61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="O61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>4512</v>
       </c>
       <c r="P61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>4244</v>
       </c>
       <c r="Q61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>4869</v>
       </c>
       <c r="R61" s="35">
@@ -4663,11 +5005,11 @@
         <v>4892</v>
       </c>
       <c r="S61" s="35">
-        <f t="shared" ref="S61" si="46">SUM(S58:S60)+S57</f>
+        <f t="shared" ref="S61" si="68">SUM(S58:S60)+S57</f>
         <v>4663</v>
       </c>
       <c r="T61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>4651</v>
       </c>
       <c r="U61" s="35">
@@ -4679,6 +5021,12 @@
       <c r="B63" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="I63" s="1">
+        <v>2427</v>
+      </c>
+      <c r="M63" s="1">
+        <v>2652</v>
+      </c>
       <c r="O63" s="1">
         <v>2930</v>
       </c>
@@ -4706,63 +5054,63 @@
         <v>116</v>
       </c>
       <c r="C64" s="35">
-        <f t="shared" ref="C64:T64" si="47">C63+C61</f>
+        <f t="shared" ref="C64:T64" si="69">C63+C61</f>
         <v>0</v>
       </c>
       <c r="D64" s="35">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="E64" s="35">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="F64" s="35">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="G64" s="35">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="H64" s="35">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="I64" s="35">
-        <f t="shared" si="47"/>
-        <v>0</v>
+        <f t="shared" si="69"/>
+        <v>6081</v>
       </c>
       <c r="J64" s="35">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="K64" s="35">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="L64" s="35">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="M64" s="35">
-        <f t="shared" si="47"/>
-        <v>0</v>
+        <f t="shared" si="69"/>
+        <v>7018</v>
       </c>
       <c r="N64" s="35">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="O64" s="35">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>7442</v>
       </c>
       <c r="P64" s="35">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>7585</v>
       </c>
       <c r="Q64" s="35">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>8211</v>
       </c>
       <c r="R64" s="35">
@@ -4770,11 +5118,11 @@
         <v>8135</v>
       </c>
       <c r="S64" s="35">
-        <f t="shared" ref="S64" si="48">S63+S61</f>
+        <f t="shared" ref="S64" si="70">S63+S61</f>
         <v>7878</v>
       </c>
       <c r="T64" s="35">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>7868</v>
       </c>
       <c r="U64" s="35">
@@ -4786,12 +5134,20 @@
       <c r="B66" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="I66" s="35">
+        <f t="shared" ref="I66" si="71">I51-I61</f>
+        <v>2967</v>
+      </c>
+      <c r="M66" s="35">
+        <f t="shared" ref="M66:O66" si="72">M51-M61</f>
+        <v>2652</v>
+      </c>
       <c r="O66" s="35">
-        <f t="shared" ref="O66:P66" si="49">O51-O61</f>
+        <f t="shared" si="72"/>
         <v>2930</v>
       </c>
       <c r="P66" s="35">
-        <f t="shared" ref="P66:Q66" si="50">P51-P61</f>
+        <f t="shared" ref="P66" si="73">P51-P61</f>
         <v>3341</v>
       </c>
       <c r="Q66" s="35">
@@ -4803,11 +5159,11 @@
         <v>3243</v>
       </c>
       <c r="S66" s="35">
-        <f t="shared" ref="S66:T66" si="51">S51-S61</f>
+        <f t="shared" ref="S66" si="74">S51-S61</f>
         <v>3215</v>
       </c>
       <c r="T66" s="35">
-        <f t="shared" ref="T66:U66" si="52">T51-T61</f>
+        <f t="shared" ref="T66" si="75">T51-T61</f>
         <v>3217</v>
       </c>
       <c r="U66" s="35">
@@ -4819,12 +5175,20 @@
       <c r="B67" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="I67" s="1">
+        <f t="shared" ref="I67" si="76">I66/I19</f>
+        <v>27.754911131898968</v>
+      </c>
+      <c r="M67" s="1">
+        <f t="shared" ref="M67:O67" si="77">M66/M19</f>
+        <v>25.402298850574713</v>
+      </c>
       <c r="O67" s="1">
-        <f t="shared" ref="O67" si="53">O66/O19</f>
+        <f t="shared" si="77"/>
         <v>28.281853281853284</v>
       </c>
       <c r="P67" s="1">
-        <f t="shared" ref="P67" si="54">P66/P19</f>
+        <f t="shared" ref="P67" si="78">P66/P19</f>
         <v>32.186897880539497</v>
       </c>
       <c r="Q67" s="1">
@@ -4832,15 +5196,15 @@
         <v>32.383720930232556</v>
       </c>
       <c r="R67" s="1">
-        <f t="shared" ref="R67:S67" si="55">R66/R19</f>
+        <f t="shared" ref="R67:S67" si="79">R66/R19</f>
         <v>31.639024390243904</v>
       </c>
       <c r="S67" s="1">
-        <f t="shared" si="55"/>
+        <f t="shared" si="79"/>
         <v>33.454734651404792</v>
       </c>
       <c r="T67" s="1">
-        <f t="shared" ref="T67" si="56">T66/T19</f>
+        <f t="shared" ref="T67" si="80">T66/T19</f>
         <v>34.187035069075456</v>
       </c>
       <c r="U67" s="1">
@@ -4853,63 +5217,63 @@
         <v>6</v>
       </c>
       <c r="C69" s="37">
-        <f t="shared" ref="C69:T69" si="57">C41</f>
+        <f t="shared" ref="C69:T69" si="81">C41</f>
         <v>0</v>
       </c>
       <c r="D69" s="37">
-        <f t="shared" si="57"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="E69" s="37">
-        <f t="shared" si="57"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="F69" s="37">
-        <f t="shared" si="57"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="G69" s="37">
-        <f t="shared" si="57"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="H69" s="37">
-        <f t="shared" si="57"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="I69" s="37">
-        <f t="shared" si="57"/>
-        <v>0</v>
+        <f t="shared" si="81"/>
+        <v>744</v>
       </c>
       <c r="J69" s="37">
-        <f t="shared" si="57"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="K69" s="37">
-        <f t="shared" si="57"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="L69" s="37">
-        <f t="shared" si="57"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="M69" s="37">
-        <f t="shared" si="57"/>
-        <v>0</v>
+        <f t="shared" si="81"/>
+        <v>1393</v>
       </c>
       <c r="N69" s="37">
-        <f t="shared" si="57"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="O69" s="37">
-        <f t="shared" si="57"/>
+        <f t="shared" si="81"/>
         <v>1963</v>
       </c>
       <c r="P69" s="37">
-        <f t="shared" si="57"/>
+        <f t="shared" si="81"/>
         <v>1845</v>
       </c>
       <c r="Q69" s="37">
-        <f t="shared" si="57"/>
+        <f t="shared" si="81"/>
         <v>1339</v>
       </c>
       <c r="R69" s="37">
@@ -4917,82 +5281,82 @@
         <v>804</v>
       </c>
       <c r="S69" s="37">
-        <f t="shared" ref="S69" si="58">S41</f>
+        <f t="shared" ref="S69" si="82">S41</f>
         <v>551</v>
       </c>
       <c r="T69" s="37">
-        <f t="shared" si="57"/>
+        <f t="shared" si="81"/>
         <v>386</v>
       </c>
       <c r="U69" s="37">
         <f>U41</f>
         <v>351</v>
       </c>
-      <c r="V69" s="66"/>
-      <c r="AI69" s="66"/>
+      <c r="V69" s="54"/>
+      <c r="AI69" s="54"/>
     </row>
     <row r="70" spans="2:35" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B70" s="32" t="s">
         <v>7</v>
       </c>
       <c r="C70" s="37">
-        <f t="shared" ref="C70:T70" si="59">C55+C58</f>
+        <f t="shared" ref="C70:T70" si="83">C55+C58</f>
         <v>0</v>
       </c>
       <c r="D70" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="E70" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="F70" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="G70" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="H70" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="I70" s="37">
-        <f t="shared" si="59"/>
-        <v>0</v>
+        <f t="shared" si="83"/>
+        <v>122</v>
       </c>
       <c r="J70" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="K70" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="L70" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="M70" s="37">
-        <f t="shared" si="59"/>
-        <v>0</v>
+        <f t="shared" si="83"/>
+        <v>131</v>
       </c>
       <c r="N70" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="O70" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>109</v>
       </c>
       <c r="P70" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>112</v>
       </c>
       <c r="Q70" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>560</v>
       </c>
       <c r="R70" s="37">
@@ -5000,82 +5364,82 @@
         <v>457</v>
       </c>
       <c r="S70" s="37">
-        <f t="shared" ref="S70" si="60">S55+S58</f>
+        <f t="shared" ref="S70" si="84">S55+S58</f>
         <v>456</v>
       </c>
       <c r="T70" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>455</v>
       </c>
       <c r="U70" s="37">
         <f>U55+U58</f>
         <v>454</v>
       </c>
-      <c r="V70" s="66"/>
-      <c r="AI70" s="66"/>
+      <c r="V70" s="54"/>
+      <c r="AI70" s="54"/>
     </row>
     <row r="71" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C71" s="35">
-        <f t="shared" ref="C71:T71" si="61">C69-C70</f>
+        <f t="shared" ref="C71:T71" si="85">C69-C70</f>
         <v>0</v>
       </c>
       <c r="D71" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="E71" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="F71" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="G71" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="H71" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="I71" s="35">
-        <f t="shared" si="61"/>
-        <v>0</v>
+        <f t="shared" si="85"/>
+        <v>622</v>
       </c>
       <c r="J71" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="K71" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="L71" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="M71" s="35">
-        <f t="shared" si="61"/>
-        <v>0</v>
+        <f t="shared" si="85"/>
+        <v>1262</v>
       </c>
       <c r="N71" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="O71" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="85"/>
         <v>1854</v>
       </c>
       <c r="P71" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="85"/>
         <v>1733</v>
       </c>
       <c r="Q71" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="85"/>
         <v>779</v>
       </c>
       <c r="R71" s="35">
@@ -5083,11 +5447,11 @@
         <v>347</v>
       </c>
       <c r="S71" s="35">
-        <f t="shared" ref="S71" si="62">S69-S70</f>
+        <f t="shared" ref="S71" si="86">S69-S70</f>
         <v>95</v>
       </c>
       <c r="T71" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="85"/>
         <v>-69</v>
       </c>
       <c r="U71" s="35">
@@ -5099,8 +5463,16 @@
       <c r="B73" s="2" t="s">
         <v>119</v>
       </c>
+      <c r="M73" s="30">
+        <f t="shared" ref="M73" si="87">M42/I42-1</f>
+        <v>-8.5122699386503076E-2</v>
+      </c>
+      <c r="Q73" s="30">
+        <f t="shared" ref="Q73:S73" si="88">Q42/M42-1</f>
+        <v>9.0528080469404859E-2</v>
+      </c>
       <c r="S73" s="30">
-        <f t="shared" ref="S73" si="63">S42/O42-1</f>
+        <f t="shared" si="88"/>
         <v>0.37218413320274246</v>
       </c>
       <c r="T73" s="30">
@@ -5117,7 +5489,7 @@
         <v>122</v>
       </c>
       <c r="P74" s="30">
-        <f t="shared" ref="P74:Q74" si="64">P42/O42-1</f>
+        <f t="shared" ref="P74" si="89">P42/O42-1</f>
         <v>5.8765915768854038E-2</v>
       </c>
       <c r="Q74" s="30">
@@ -5129,34 +5501,34 @@
         <v>-2.6902382782475032E-2</v>
       </c>
       <c r="S74" s="30">
-        <f t="shared" ref="S74:U74" si="65">S42/R42-1</f>
+        <f t="shared" ref="S74:T74" si="90">S42/R42-1</f>
         <v>0.10663507109004744</v>
       </c>
       <c r="T74" s="30">
-        <f t="shared" si="65"/>
+        <f t="shared" si="90"/>
         <v>0.17344753747323338</v>
       </c>
       <c r="U74" s="30">
         <f>U42/T42-1</f>
         <v>2.4939172749391725E-2</v>
       </c>
-      <c r="V74" s="68"/>
-      <c r="AI74" s="68"/>
+      <c r="V74" s="56"/>
+      <c r="AI74" s="56"/>
     </row>
     <row r="75" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B75" s="1" t="s">
         <v>120</v>
       </c>
       <c r="R75" s="30">
-        <f t="shared" ref="R75:T75" si="66">R42/SUM(O6:R6)</f>
+        <f t="shared" ref="R75:T75" si="91">R42/SUM(O6:R6)</f>
         <v>0.14132618888144674</v>
       </c>
       <c r="S75" s="30">
-        <f t="shared" si="66"/>
+        <f t="shared" si="91"/>
         <v>0.15601336302895322</v>
       </c>
       <c r="T75" s="30">
-        <f t="shared" si="66"/>
+        <f t="shared" si="91"/>
         <v>0.18745724059293045</v>
       </c>
       <c r="U75" s="30">
@@ -5195,11 +5567,11 @@
         <v>5</v>
       </c>
       <c r="O78" s="35">
-        <f t="shared" ref="O78" si="67">O77*O19</f>
+        <f t="shared" ref="O78" si="92">O77*O19</f>
         <v>6119.652</v>
       </c>
       <c r="P78" s="35">
-        <f t="shared" ref="P78" si="68">P77*P19</f>
+        <f t="shared" ref="P78" si="93">P77*P19</f>
         <v>5546.0339999999997</v>
       </c>
       <c r="Q78" s="35">
@@ -5207,15 +5579,15 @@
         <v>4635.7440000000006</v>
       </c>
       <c r="R78" s="35">
-        <f t="shared" ref="R78" si="69">R77*R19</f>
+        <f t="shared" ref="R78" si="94">R77*R19</f>
         <v>4321.3999999999996</v>
       </c>
       <c r="S78" s="35">
-        <f t="shared" ref="S78" si="70">S77*S19</f>
+        <f t="shared" ref="S78" si="95">S77*S19</f>
         <v>2710.02</v>
       </c>
       <c r="T78" s="35">
-        <f t="shared" ref="T78" si="71">T77*T19</f>
+        <f t="shared" ref="T78" si="96">T77*T19</f>
         <v>2610.3339999999998</v>
       </c>
       <c r="U78" s="35">
@@ -5228,11 +5600,11 @@
         <v>9</v>
       </c>
       <c r="O79" s="35">
-        <f t="shared" ref="O79" si="72">O78-O71</f>
+        <f t="shared" ref="O79" si="97">O78-O71</f>
         <v>4265.652</v>
       </c>
       <c r="P79" s="35">
-        <f t="shared" ref="P79" si="73">P78-P71</f>
+        <f t="shared" ref="P79" si="98">P78-P71</f>
         <v>3813.0339999999997</v>
       </c>
       <c r="Q79" s="35">
@@ -5240,15 +5612,15 @@
         <v>3856.7440000000006</v>
       </c>
       <c r="R79" s="35">
-        <f t="shared" ref="R79" si="74">R78-R71</f>
+        <f t="shared" ref="R79" si="99">R78-R71</f>
         <v>3974.3999999999996</v>
       </c>
       <c r="S79" s="35">
-        <f t="shared" ref="S79" si="75">S78-S71</f>
+        <f t="shared" ref="S79" si="100">S78-S71</f>
         <v>2615.02</v>
       </c>
       <c r="T79" s="35">
-        <f t="shared" ref="T79" si="76">T78-T71</f>
+        <f t="shared" ref="T79" si="101">T78-T71</f>
         <v>2679.3339999999998</v>
       </c>
       <c r="U79" s="35">
@@ -5261,11 +5633,11 @@
         <v>22</v>
       </c>
       <c r="O81" s="33">
-        <f t="shared" ref="O81:P81" si="77">O77/O67</f>
+        <f t="shared" ref="O81" si="102">O77/O67</f>
         <v>2.0886184300341295</v>
       </c>
       <c r="P81" s="33">
-        <f t="shared" ref="P81:Q81" si="78">P77/P67</f>
+        <f t="shared" ref="P81" si="103">P77/P67</f>
         <v>1.6599922178988327</v>
       </c>
       <c r="Q81" s="33">
@@ -5273,23 +5645,23 @@
         <v>1.387116696588869</v>
       </c>
       <c r="R81" s="33">
-        <f t="shared" ref="R81:S81" si="79">R77/R67</f>
+        <f t="shared" ref="R81" si="104">R77/R67</f>
         <v>1.3325316065371569</v>
       </c>
       <c r="S81" s="33">
-        <f t="shared" ref="S81:T81" si="80">S77/S67</f>
+        <f t="shared" ref="S81" si="105">S77/S67</f>
         <v>0.84293001555209934</v>
       </c>
       <c r="T81" s="33">
-        <f t="shared" ref="T81:U81" si="81">T77/T67</f>
+        <f t="shared" ref="T81" si="106">T77/T67</f>
         <v>0.81141871308672664</v>
       </c>
       <c r="U81" s="33">
         <f>U77/U67</f>
         <v>0.8912979441546488</v>
       </c>
-      <c r="V81" s="73"/>
-      <c r="AI81" s="73"/>
+      <c r="V81" s="61"/>
+      <c r="AI81" s="61"/>
     </row>
     <row r="82" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B82" s="1" t="s">
@@ -5306,15 +5678,15 @@
         <v>25</v>
       </c>
       <c r="R84" s="33">
-        <f t="shared" ref="R84:T84" si="82">R77/SUM(O18:R18)</f>
+        <f t="shared" ref="R84:T84" si="107">R77/SUM(O18:R18)</f>
         <v>4.8917919939957191</v>
       </c>
       <c r="S84" s="33">
-        <f t="shared" si="82"/>
+        <f t="shared" si="107"/>
         <v>3.5064679704443651</v>
       </c>
       <c r="T84" s="33">
-        <f t="shared" si="82"/>
+        <f t="shared" si="107"/>
         <v>5.662800594373258</v>
       </c>
       <c r="U84" s="33">
@@ -5339,14 +5711,16 @@
     <hyperlink ref="S1" r:id="rId3" xr:uid="{BC742AC0-9220-4959-A8E6-12B999B89343}"/>
     <hyperlink ref="R1" r:id="rId4" xr:uid="{6F70B379-E793-4F12-B06A-982457527E59}"/>
     <hyperlink ref="AH1" r:id="rId5" xr:uid="{38A8ED3A-2717-4FEA-BB5C-B793AAB5C38B}"/>
+    <hyperlink ref="M1" r:id="rId6" xr:uid="{43A5C21D-F886-4FCB-A94B-86147CFAE126}"/>
+    <hyperlink ref="L1" r:id="rId7" xr:uid="{9446438F-F601-4E14-BBC3-368E3CAEABAA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId8"/>
   <ignoredErrors>
     <ignoredError sqref="R6:R17 V12 AI8:AI15 AI16:AI19" formula="1"/>
     <ignoredError sqref="AH8 AH15 AH12" formula="1" formulaRange="1"/>
     <ignoredError sqref="AH17" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
$FL more historical results
</commit_message>
<xml_diff>
--- a/$FL.xlsx
+++ b/$FL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AC89D7-DBE9-4A6B-B976-25816F1037C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54CF69F-F907-4B66-A8A4-4562DC3E08B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{77D9C7A4-F0C3-486A-8AA0-E7E6A2714164}"/>
   </bookViews>
@@ -788,6 +788,8 @@
     <xf numFmtId="9" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,7 +802,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -818,14 +823,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1315,7 +1315,7 @@
   <dimension ref="A2:Q41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:D31"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1334,24 +1334,24 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="73"/>
-      <c r="G5" s="71" t="s">
+      <c r="C5" s="75"/>
+      <c r="D5" s="76"/>
+      <c r="G5" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="73"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="76"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
@@ -1537,11 +1537,11 @@
       <c r="Q14" s="7"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B15" s="71" t="s">
+      <c r="B15" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="72"/>
-      <c r="D15" s="73"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="76"/>
       <c r="G15" s="15"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -1558,10 +1558,10 @@
       <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="68" t="s">
+      <c r="C16" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="69"/>
+      <c r="D16" s="71"/>
       <c r="G16" s="15"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1581,10 +1581,10 @@
       <c r="B17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="69"/>
+      <c r="D17" s="71"/>
       <c r="G17" s="15"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -1604,10 +1604,10 @@
       <c r="B18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="69"/>
+      <c r="D18" s="71"/>
       <c r="G18" s="15"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -1624,10 +1624,10 @@
       <c r="B19" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="76" t="s">
+      <c r="C19" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="77"/>
+      <c r="D19" s="73"/>
       <c r="G19" s="15"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -1667,11 +1667,11 @@
       <c r="Q21" s="7"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="72"/>
-      <c r="D22" s="73"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="76"/>
       <c r="G22" s="15"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -1688,10 +1688,10 @@
       <c r="B23" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="68" t="s">
+      <c r="C23" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="69"/>
+      <c r="D23" s="71"/>
       <c r="G23" s="15"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -1708,10 +1708,10 @@
       <c r="B24" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="68">
+      <c r="C24" s="70">
         <v>1879</v>
       </c>
-      <c r="D24" s="69"/>
+      <c r="D24" s="71"/>
       <c r="G24" s="15"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -1728,11 +1728,11 @@
       <c r="B25" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="70">
+      <c r="C25" s="79">
         <f>'Financial Model'!U33</f>
         <v>2794</v>
       </c>
-      <c r="D25" s="69"/>
+      <c r="D25" s="71"/>
       <c r="G25" s="15"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -1747,8 +1747,8 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B26" s="13"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="69"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="71"/>
       <c r="G26" s="15"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -1765,11 +1765,11 @@
       <c r="B27" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="70">
+      <c r="C27" s="79">
         <f>'Financial Model'!U33</f>
         <v>2794</v>
       </c>
-      <c r="D27" s="69"/>
+      <c r="D27" s="71"/>
       <c r="G27" s="15"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -1786,11 +1786,11 @@
       <c r="B28" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="70">
+      <c r="C28" s="79">
         <f>'Financial Model'!U42</f>
         <v>1685</v>
       </c>
-      <c r="D28" s="69"/>
+      <c r="D28" s="71"/>
       <c r="G28" s="15"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -1805,8 +1805,8 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B29" s="13"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="69"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="71"/>
       <c r="G29" s="15"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -1846,10 +1846,10 @@
       <c r="B31" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="74" t="s">
+      <c r="C31" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="75"/>
+      <c r="D31" s="78"/>
       <c r="G31" s="16"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
@@ -1863,81 +1863,83 @@
       <c r="Q31" s="9"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="71" t="s">
+      <c r="B34" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="72"/>
-      <c r="D34" s="73"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="76"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="66">
+      <c r="C35" s="68">
         <f>C6/'Financial Model'!U67</f>
         <v>1.1231500460263886</v>
       </c>
-      <c r="D35" s="67"/>
+      <c r="D35" s="69"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="66">
+      <c r="C36" s="68">
         <f>C8/SUM('Financial Model'!R6:U6)</f>
         <v>0.41777787687114459</v>
       </c>
-      <c r="D36" s="67"/>
+      <c r="D36" s="69"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="66">
+      <c r="C37" s="68">
         <f>C12/SUM('Financial Model'!R6:U6)</f>
         <v>0.42954392667694763</v>
       </c>
-      <c r="D37" s="67"/>
+      <c r="D37" s="69"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="66">
+      <c r="C38" s="68">
         <f>C6/SUM('Financial Model'!R18:U18)</f>
         <v>8.9160063090667094</v>
       </c>
-      <c r="D38" s="67"/>
+      <c r="D38" s="69"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="66">
+      <c r="C39" s="68">
         <f>C12/SUM('Financial Model'!R17:U17)</f>
         <v>8.8684611654009426</v>
       </c>
-      <c r="D39" s="67"/>
+      <c r="D39" s="69"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="68"/>
-      <c r="D40" s="69"/>
+      <c r="C40" s="70"/>
+      <c r="D40" s="71"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="14"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="77"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="G5:Q5"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C31:D31"/>
@@ -1950,13 +1952,11 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C31:D31" r:id="rId1" display="Link" xr:uid="{895B3114-FB4F-46F5-A7E6-2022E34FF531}"/>
@@ -1975,7 +1975,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I26" sqref="H26:I29"/>
+      <selection pane="bottomRight" activeCell="P35" sqref="N35:P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2014,7 +2014,7 @@
       <c r="J1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="23" t="s">
         <v>37</v>
       </c>
       <c r="L1" s="23" t="s">
@@ -2119,18 +2119,28 @@
     </row>
     <row r="2" spans="1:46" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25"/>
+      <c r="G2" s="27">
+        <v>43589</v>
+      </c>
       <c r="H2" s="27">
         <v>43680</v>
       </c>
       <c r="I2" s="27">
         <v>43771</v>
       </c>
+      <c r="K2" s="27">
+        <v>43953</v>
+      </c>
       <c r="L2" s="27">
         <v>44044</v>
       </c>
       <c r="M2" s="27">
         <v>44135</v>
       </c>
+      <c r="N2" s="27">
+        <f>AG2</f>
+        <v>44226</v>
+      </c>
       <c r="O2" s="27">
         <v>44317</v>
       </c>
@@ -2167,6 +2177,9 @@
     </row>
     <row r="3" spans="1:46" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25"/>
+      <c r="K3" s="45">
+        <v>44682</v>
+      </c>
       <c r="L3" s="45">
         <v>44409</v>
       </c>
@@ -2199,7 +2212,9 @@
       <c r="D4" s="37"/>
       <c r="E4" s="37"/>
       <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="G4" s="37">
+        <v>1758</v>
+      </c>
       <c r="H4" s="37">
         <v>1521</v>
       </c>
@@ -2207,14 +2222,19 @@
         <v>1636</v>
       </c>
       <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
+      <c r="K4" s="37">
+        <v>814</v>
+      </c>
       <c r="L4" s="37">
         <v>1388</v>
       </c>
       <c r="M4" s="37">
         <v>1656</v>
       </c>
-      <c r="N4" s="37"/>
+      <c r="N4" s="37">
+        <f>AG4-SUM(K4:M4)</f>
+        <v>1589</v>
+      </c>
       <c r="O4" s="37">
         <v>1620</v>
       </c>
@@ -2256,7 +2276,9 @@
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="G5" s="37">
+        <v>320</v>
+      </c>
       <c r="H5" s="37">
         <v>253</v>
       </c>
@@ -2264,14 +2286,19 @@
         <v>296</v>
       </c>
       <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
+      <c r="K5" s="37">
+        <v>362</v>
+      </c>
       <c r="L5" s="37">
         <v>689</v>
       </c>
       <c r="M5" s="37">
         <v>450</v>
       </c>
-      <c r="N5" s="37"/>
+      <c r="N5" s="37">
+        <f>AG5-SUM(K5:M5)</f>
+        <v>600</v>
+      </c>
       <c r="O5" s="37">
         <v>533</v>
       </c>
@@ -2313,9 +2340,12 @@
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
       <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
+      <c r="G6" s="34">
+        <f t="shared" ref="G6:I6" si="0">G4+G5</f>
+        <v>2078</v>
+      </c>
       <c r="H6" s="34">
-        <f t="shared" ref="H6:I6" si="0">H4+H5</f>
+        <f t="shared" si="0"/>
         <v>1774</v>
       </c>
       <c r="I6" s="34">
@@ -2323,16 +2353,22 @@
         <v>1932</v>
       </c>
       <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
+      <c r="K6" s="34">
+        <f t="shared" ref="K6:U6" si="1">K4+K5</f>
+        <v>1176</v>
+      </c>
       <c r="L6" s="34">
-        <f t="shared" ref="L6:U6" si="1">L4+L5</f>
+        <f t="shared" si="1"/>
         <v>2077</v>
       </c>
       <c r="M6" s="34">
         <f t="shared" si="1"/>
         <v>2106</v>
       </c>
-      <c r="N6" s="34"/>
+      <c r="N6" s="34">
+        <f t="shared" si="1"/>
+        <v>2189</v>
+      </c>
       <c r="O6" s="34">
         <f t="shared" si="1"/>
         <v>2153</v>
@@ -2379,6 +2415,10 @@
         <f>SUM(S6:V6)</f>
         <v>8694.65</v>
       </c>
+      <c r="AJ6" s="34">
+        <f>AI6*(1+AJ21)</f>
+        <v>9042.4359999999997</v>
+      </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -2388,7 +2428,9 @@
       <c r="D7" s="35"/>
       <c r="E7" s="35"/>
       <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
+      <c r="G7" s="35">
+        <v>1389</v>
+      </c>
       <c r="H7" s="35">
         <v>1240</v>
       </c>
@@ -2396,14 +2438,19 @@
         <v>1312</v>
       </c>
       <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
+      <c r="K7" s="35">
+        <v>905</v>
+      </c>
       <c r="L7" s="35">
         <v>1539</v>
       </c>
       <c r="M7" s="35">
         <v>1456</v>
       </c>
-      <c r="N7" s="35"/>
+      <c r="N7" s="35">
+        <f>AG7-SUM(K7:M7)</f>
+        <v>1465</v>
+      </c>
       <c r="O7" s="35">
         <v>1404</v>
       </c>
@@ -2442,6 +2489,10 @@
         <f>SUM(S7:V7)</f>
         <v>5874.5219999999999</v>
       </c>
+      <c r="AJ7" s="35">
+        <f>AJ6-AJ8</f>
+        <v>5968.0077599999995</v>
+      </c>
     </row>
     <row r="8" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
@@ -2465,7 +2516,7 @@
       </c>
       <c r="G8" s="34">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>689</v>
       </c>
       <c r="H8" s="34">
         <f t="shared" si="2"/>
@@ -2481,7 +2532,7 @@
       </c>
       <c r="K8" s="34">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>271</v>
       </c>
       <c r="L8" s="34">
         <f t="shared" si="2"/>
@@ -2493,7 +2544,7 @@
       </c>
       <c r="N8" s="34">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>724</v>
       </c>
       <c r="O8" s="34">
         <f t="shared" si="2"/>
@@ -2528,7 +2579,7 @@
         <v>730.12800000000016</v>
       </c>
       <c r="AD8" s="34">
-        <f t="shared" ref="AD8:AE8" si="3">AD6-AD7</f>
+        <f t="shared" ref="AD8" si="3">AD6-AD7</f>
         <v>0</v>
       </c>
       <c r="AE8" s="34">
@@ -2550,6 +2601,10 @@
       <c r="AI8" s="62">
         <f>AI6-AI7</f>
         <v>2820.1279999999997</v>
+      </c>
+      <c r="AJ8" s="34">
+        <f>AJ6*AJ26</f>
+        <v>3074.4282400000002</v>
       </c>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.2">
@@ -2560,7 +2615,9 @@
       <c r="D9" s="35"/>
       <c r="E9" s="35"/>
       <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
+      <c r="G9" s="35">
+        <v>416</v>
+      </c>
       <c r="H9" s="35">
         <v>393</v>
       </c>
@@ -2568,14 +2625,19 @@
         <v>411</v>
       </c>
       <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
+      <c r="K9" s="35">
+        <v>316</v>
+      </c>
       <c r="L9" s="35">
         <v>387</v>
       </c>
       <c r="M9" s="35">
         <v>424</v>
       </c>
-      <c r="N9" s="35"/>
+      <c r="N9" s="35">
+        <f t="shared" ref="N9:N11" si="5">AG9-SUM(K9:M9)</f>
+        <v>460</v>
+      </c>
       <c r="O9" s="35">
         <v>418</v>
       </c>
@@ -2586,7 +2648,7 @@
         <v>458</v>
       </c>
       <c r="R9" s="35">
-        <f t="shared" ref="R9:R11" si="5">AH9-SUM(O9:Q9)</f>
+        <f t="shared" ref="R9:R11" si="6">AH9-SUM(O9:Q9)</f>
         <v>525</v>
       </c>
       <c r="S9" s="35">
@@ -2616,9 +2678,14 @@
         <v>1851</v>
       </c>
       <c r="AI9" s="57">
-        <f t="shared" ref="AI9:AI11" si="6">SUM(S9:V9)</f>
+        <f t="shared" ref="AI9:AI11" si="7">SUM(S9:V9)</f>
         <v>1861.1465000000001</v>
       </c>
+      <c r="AJ9" s="35">
+        <f>AJ6*0.21</f>
+        <v>1898.9115599999998</v>
+      </c>
+      <c r="AK9" s="35"/>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
@@ -2628,7 +2695,9 @@
       <c r="D10" s="35"/>
       <c r="E10" s="35"/>
       <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="G10" s="35">
+        <v>44</v>
+      </c>
       <c r="H10" s="35">
         <v>46</v>
       </c>
@@ -2636,14 +2705,19 @@
         <v>44</v>
       </c>
       <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
+      <c r="K10" s="35">
+        <v>44</v>
+      </c>
       <c r="L10" s="35">
         <v>44</v>
       </c>
       <c r="M10" s="35">
         <v>44</v>
       </c>
-      <c r="N10" s="35"/>
+      <c r="N10" s="35">
+        <f t="shared" si="5"/>
+        <v>44</v>
+      </c>
       <c r="O10" s="35">
         <v>45</v>
       </c>
@@ -2654,7 +2728,7 @@
         <v>49</v>
       </c>
       <c r="R10" s="35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="S10" s="35">
@@ -2680,8 +2754,52 @@
         <v>197</v>
       </c>
       <c r="AI10" s="57">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>210</v>
+      </c>
+      <c r="AJ10" s="35">
+        <f>AVERAGE(AD10:AI10)</f>
+        <v>194.33333333333334</v>
+      </c>
+      <c r="AK10" s="35">
+        <f t="shared" ref="AK10:AT11" si="8">AVERAGE(AE10:AJ10)</f>
+        <v>194.33333333333334</v>
+      </c>
+      <c r="AL10" s="35">
+        <f t="shared" si="8"/>
+        <v>194.33333333333334</v>
+      </c>
+      <c r="AM10" s="35">
+        <f t="shared" si="8"/>
+        <v>194.33333333333334</v>
+      </c>
+      <c r="AN10" s="35">
+        <f t="shared" si="8"/>
+        <v>197.38888888888891</v>
+      </c>
+      <c r="AO10" s="35">
+        <f t="shared" si="8"/>
+        <v>197.45370370370372</v>
+      </c>
+      <c r="AP10" s="35">
+        <f t="shared" si="8"/>
+        <v>195.36265432098767</v>
+      </c>
+      <c r="AQ10" s="35">
+        <f t="shared" si="8"/>
+        <v>195.53420781893007</v>
+      </c>
+      <c r="AR10" s="35">
+        <f t="shared" si="8"/>
+        <v>195.73435356652951</v>
+      </c>
+      <c r="AS10" s="35">
+        <f t="shared" si="8"/>
+        <v>195.96785693872889</v>
+      </c>
+      <c r="AT10" s="35">
+        <f t="shared" si="8"/>
+        <v>196.24027753962812</v>
       </c>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.2">
@@ -2692,7 +2810,9 @@
       <c r="D11" s="35"/>
       <c r="E11" s="35"/>
       <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
+      <c r="G11" s="35">
+        <v>1</v>
+      </c>
       <c r="H11" s="35">
         <v>14</v>
       </c>
@@ -2700,14 +2820,19 @@
         <v>1</v>
       </c>
       <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
+      <c r="K11" s="35">
+        <v>16</v>
+      </c>
       <c r="L11" s="35">
         <v>38</v>
       </c>
       <c r="M11" s="35">
         <v>4</v>
       </c>
-      <c r="N11" s="35"/>
+      <c r="N11" s="35">
+        <f t="shared" si="5"/>
+        <v>59</v>
+      </c>
       <c r="O11" s="35">
         <v>4</v>
       </c>
@@ -2718,7 +2843,7 @@
         <v>57</v>
       </c>
       <c r="R11" s="35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="S11" s="35">
@@ -2744,8 +2869,52 @@
         <v>172</v>
       </c>
       <c r="AI11" s="57">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>66.25</v>
+      </c>
+      <c r="AJ11" s="35">
+        <f t="shared" ref="AJ11" si="9">AVERAGE(AD11:AI11)</f>
+        <v>118.41666666666667</v>
+      </c>
+      <c r="AK11" s="35">
+        <f t="shared" si="8"/>
+        <v>118.41666666666667</v>
+      </c>
+      <c r="AL11" s="35">
+        <f t="shared" si="8"/>
+        <v>118.41666666666667</v>
+      </c>
+      <c r="AM11" s="35">
+        <f t="shared" si="8"/>
+        <v>118.41666666666667</v>
+      </c>
+      <c r="AN11" s="35">
+        <f t="shared" si="8"/>
+        <v>118.65277777777777</v>
+      </c>
+      <c r="AO11" s="35">
+        <f t="shared" si="8"/>
+        <v>109.76157407407409</v>
+      </c>
+      <c r="AP11" s="35">
+        <f t="shared" si="8"/>
+        <v>117.01350308641976</v>
+      </c>
+      <c r="AQ11" s="35">
+        <f t="shared" si="8"/>
+        <v>116.77964248971193</v>
+      </c>
+      <c r="AR11" s="35">
+        <f t="shared" si="8"/>
+        <v>116.50680512688615</v>
+      </c>
+      <c r="AS11" s="35">
+        <f t="shared" si="8"/>
+        <v>116.18849487025606</v>
+      </c>
+      <c r="AT11" s="35">
+        <f t="shared" si="8"/>
+        <v>115.8171329041876</v>
       </c>
     </row>
     <row r="12" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2753,75 +2922,75 @@
         <v>82</v>
       </c>
       <c r="C12" s="34">
-        <f t="shared" ref="C12:T12" si="7">C8-C9-C10-C11</f>
+        <f t="shared" ref="C12:T12" si="10">C8-C9-C10-C11</f>
         <v>0</v>
       </c>
       <c r="D12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="E12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G12" s="34">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>228</v>
       </c>
       <c r="H12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>81</v>
       </c>
       <c r="I12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>164</v>
       </c>
       <c r="J12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K12" s="34">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>-105</v>
       </c>
       <c r="L12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>69</v>
       </c>
       <c r="M12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>178</v>
       </c>
       <c r="N12" s="34">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>161</v>
       </c>
       <c r="O12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>282</v>
       </c>
       <c r="P12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>264</v>
       </c>
       <c r="Q12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>196</v>
       </c>
       <c r="R12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>118</v>
       </c>
       <c r="S12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>217</v>
       </c>
       <c r="T12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>139</v>
       </c>
       <c r="U12" s="34">
@@ -2833,28 +3002,32 @@
         <v>169.73150000000015</v>
       </c>
       <c r="AD12" s="34">
-        <f t="shared" ref="AD12:AE12" si="8">AD8-AD9-AD10-AD11</f>
+        <f t="shared" ref="AD12" si="11">AD8-AD9-AD10-AD11</f>
         <v>0</v>
       </c>
       <c r="AE12" s="34">
-        <f t="shared" ref="AE12:AI12" si="9">AE8-AE9-AE10-AE11</f>
+        <f t="shared" ref="AE12:AJ12" si="12">AE8-AE9-AE10-AE11</f>
         <v>0</v>
       </c>
       <c r="AF12" s="34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AG12" s="34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>303</v>
       </c>
       <c r="AH12" s="34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>860</v>
       </c>
       <c r="AI12" s="62">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>682.73149999999964</v>
+      </c>
+      <c r="AJ12" s="34">
+        <f t="shared" si="12"/>
+        <v>862.76668000000041</v>
       </c>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.2">
@@ -2865,7 +3038,9 @@
       <c r="D13" s="35"/>
       <c r="E13" s="35"/>
       <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
+      <c r="G13" s="35">
+        <v>4</v>
+      </c>
       <c r="H13" s="35">
         <v>2</v>
       </c>
@@ -2873,14 +3048,19 @@
         <v>3</v>
       </c>
       <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
+      <c r="K13" s="35">
+        <v>-1</v>
+      </c>
       <c r="L13" s="35">
         <v>-2</v>
       </c>
       <c r="M13" s="35">
         <v>-2</v>
       </c>
-      <c r="N13" s="35"/>
+      <c r="N13" s="35">
+        <f t="shared" ref="N13:N14" si="13">AG13-SUM(K13:M13)</f>
+        <v>-2</v>
+      </c>
       <c r="O13" s="35">
         <v>-2</v>
       </c>
@@ -2891,7 +3071,7 @@
         <v>-4</v>
       </c>
       <c r="R13" s="35">
-        <f t="shared" ref="R13:R14" si="10">AH13-SUM(O13:Q13)</f>
+        <f t="shared" ref="R13:R14" si="14">AH13-SUM(O13:Q13)</f>
         <v>-6</v>
       </c>
       <c r="S13" s="35">
@@ -2917,8 +3097,52 @@
         <v>-14</v>
       </c>
       <c r="AI13" s="57">
-        <f t="shared" ref="AI13:AI14" si="11">SUM(S13:V13)</f>
+        <f t="shared" ref="AI13:AI14" si="15">SUM(S13:V13)</f>
         <v>-17.75</v>
+      </c>
+      <c r="AJ13" s="35">
+        <f t="shared" ref="AJ13:AJ14" si="16">AVERAGE(AD13:AI13)</f>
+        <v>-12.916666666666666</v>
+      </c>
+      <c r="AK13" s="35">
+        <f t="shared" ref="AK13:AK14" si="17">AVERAGE(AE13:AJ13)</f>
+        <v>-12.916666666666666</v>
+      </c>
+      <c r="AL13" s="35">
+        <f t="shared" ref="AL13:AL14" si="18">AVERAGE(AF13:AK13)</f>
+        <v>-12.916666666666666</v>
+      </c>
+      <c r="AM13" s="35">
+        <f t="shared" ref="AM13:AM14" si="19">AVERAGE(AG13:AL13)</f>
+        <v>-12.916666666666666</v>
+      </c>
+      <c r="AN13" s="35">
+        <f t="shared" ref="AN13:AN14" si="20">AVERAGE(AH13:AM13)</f>
+        <v>-13.902777777777779</v>
+      </c>
+      <c r="AO13" s="35">
+        <f t="shared" ref="AO13:AO14" si="21">AVERAGE(AI13:AN13)</f>
+        <v>-13.886574074074071</v>
+      </c>
+      <c r="AP13" s="35">
+        <f t="shared" ref="AP13:AP14" si="22">AVERAGE(AJ13:AO13)</f>
+        <v>-13.242669753086419</v>
+      </c>
+      <c r="AQ13" s="35">
+        <f t="shared" ref="AQ13:AQ14" si="23">AVERAGE(AK13:AP13)</f>
+        <v>-13.297003600823045</v>
+      </c>
+      <c r="AR13" s="35">
+        <f t="shared" ref="AR13:AR14" si="24">AVERAGE(AL13:AQ13)</f>
+        <v>-13.36039308984911</v>
+      </c>
+      <c r="AS13" s="35">
+        <f t="shared" ref="AS13:AS14" si="25">AVERAGE(AM13:AR13)</f>
+        <v>-13.434347493712847</v>
+      </c>
+      <c r="AT13" s="35">
+        <f t="shared" ref="AT13:AT14" si="26">AVERAGE(AN13:AS13)</f>
+        <v>-13.520627631553879</v>
       </c>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.2">
@@ -2929,7 +3153,9 @@
       <c r="D14" s="35"/>
       <c r="E14" s="35"/>
       <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
+      <c r="G14" s="35">
+        <v>2</v>
+      </c>
       <c r="H14" s="35">
         <v>2</v>
       </c>
@@ -2937,14 +3163,19 @@
         <v>4</v>
       </c>
       <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
+      <c r="K14" s="35">
+        <v>1</v>
+      </c>
       <c r="L14" s="35">
         <v>3</v>
       </c>
       <c r="M14" s="35">
         <v>193</v>
       </c>
-      <c r="N14" s="35"/>
+      <c r="N14" s="35">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
       <c r="O14" s="35">
         <v>4</v>
       </c>
@@ -2955,7 +3186,7 @@
         <v>30</v>
       </c>
       <c r="R14" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>35</v>
       </c>
       <c r="S14" s="35">
@@ -2981,8 +3212,52 @@
         <v>394</v>
       </c>
       <c r="AI14" s="57">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>-21.25</v>
+      </c>
+      <c r="AJ14" s="35">
+        <f t="shared" si="16"/>
+        <v>190.25</v>
+      </c>
+      <c r="AK14" s="35">
+        <f t="shared" si="17"/>
+        <v>190.25</v>
+      </c>
+      <c r="AL14" s="35">
+        <f t="shared" si="18"/>
+        <v>190.25</v>
+      </c>
+      <c r="AM14" s="35">
+        <f t="shared" si="19"/>
+        <v>190.25</v>
+      </c>
+      <c r="AN14" s="35">
+        <f t="shared" si="20"/>
+        <v>188.95833333333334</v>
+      </c>
+      <c r="AO14" s="35">
+        <f t="shared" si="21"/>
+        <v>154.78472222222223</v>
+      </c>
+      <c r="AP14" s="35">
+        <f t="shared" si="22"/>
+        <v>184.12384259259261</v>
+      </c>
+      <c r="AQ14" s="35">
+        <f t="shared" si="23"/>
+        <v>183.10281635802471</v>
+      </c>
+      <c r="AR14" s="35">
+        <f t="shared" si="24"/>
+        <v>181.91161908436217</v>
+      </c>
+      <c r="AS14" s="35">
+        <f t="shared" si="25"/>
+        <v>180.52188893175585</v>
+      </c>
+      <c r="AT14" s="35">
+        <f t="shared" si="26"/>
+        <v>178.90053708704849</v>
       </c>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.2">
@@ -2990,75 +3265,75 @@
         <v>85</v>
       </c>
       <c r="C15" s="35">
-        <f t="shared" ref="C15:T15" si="12">C12+C13+C14</f>
+        <f t="shared" ref="C15:T15" si="27">C12+C13+C14</f>
         <v>0</v>
       </c>
       <c r="D15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="F15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="G15" s="35">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>234</v>
       </c>
       <c r="H15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>85</v>
       </c>
       <c r="I15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>171</v>
       </c>
       <c r="J15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="K15" s="35">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>-105</v>
       </c>
       <c r="L15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>70</v>
       </c>
       <c r="M15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>369</v>
       </c>
       <c r="N15" s="35">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>160</v>
       </c>
       <c r="O15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>284</v>
       </c>
       <c r="P15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>587</v>
       </c>
       <c r="Q15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>222</v>
       </c>
       <c r="R15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>147</v>
       </c>
       <c r="S15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>190</v>
       </c>
       <c r="T15" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>143</v>
       </c>
       <c r="U15" s="35">
@@ -3070,28 +3345,32 @@
         <v>167.73150000000015</v>
       </c>
       <c r="AD15" s="35">
-        <f t="shared" ref="AD15:AE15" si="13">AD12+AD13+AD14</f>
+        <f t="shared" ref="AD15" si="28">AD12+AD13+AD14</f>
         <v>0</v>
       </c>
       <c r="AE15" s="35">
-        <f t="shared" ref="AE15:AI15" si="14">AE12+AE13+AE14</f>
+        <f t="shared" ref="AE15:AJ15" si="29">AE12+AE13+AE14</f>
         <v>0</v>
       </c>
       <c r="AF15" s="35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AG15" s="35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>494</v>
       </c>
       <c r="AH15" s="35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>1240</v>
       </c>
       <c r="AI15" s="57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>643.73149999999964</v>
+      </c>
+      <c r="AJ15" s="35">
+        <f t="shared" si="29"/>
+        <v>1040.1000133333337</v>
       </c>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.2">
@@ -3102,7 +3381,9 @@
       <c r="D16" s="35"/>
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
+      <c r="G16" s="35">
+        <v>62</v>
+      </c>
       <c r="H16" s="35">
         <v>25</v>
       </c>
@@ -3110,14 +3391,19 @@
         <v>46</v>
       </c>
       <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
+      <c r="K16" s="35">
+        <v>5</v>
+      </c>
       <c r="L16" s="35">
         <v>25</v>
       </c>
       <c r="M16" s="35">
         <v>104</v>
       </c>
-      <c r="N16" s="35"/>
+      <c r="N16" s="35">
+        <f>AG16-SUM(K16:M16)</f>
+        <v>37</v>
+      </c>
       <c r="O16" s="35">
         <v>82</v>
       </c>
@@ -3157,81 +3443,85 @@
         <f>SUM(S16:V16)</f>
         <v>209.35139500000005</v>
       </c>
-    </row>
-    <row r="17" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AJ16" s="35">
+        <f>AJ15*AJ29</f>
+        <v>312.03000400000008</v>
+      </c>
+    </row>
+    <row r="17" spans="2:46" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C17" s="34">
-        <f t="shared" ref="C17:T17" si="15">C15-C16</f>
+        <f t="shared" ref="C17:T17" si="30">C15-C16</f>
         <v>0</v>
       </c>
       <c r="D17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="E17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="F17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="G17" s="34">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f t="shared" si="30"/>
+        <v>172</v>
       </c>
       <c r="H17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>60</v>
       </c>
       <c r="I17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>125</v>
       </c>
       <c r="J17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="K17" s="34">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f t="shared" si="30"/>
+        <v>-110</v>
       </c>
       <c r="L17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>45</v>
       </c>
       <c r="M17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>265</v>
       </c>
       <c r="N17" s="34">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f t="shared" si="30"/>
+        <v>123</v>
       </c>
       <c r="O17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>202</v>
       </c>
       <c r="P17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>430</v>
       </c>
       <c r="Q17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>158</v>
       </c>
       <c r="R17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>102</v>
       </c>
       <c r="S17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>132</v>
       </c>
       <c r="T17" s="34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>94</v>
       </c>
       <c r="U17" s="34">
@@ -3244,31 +3534,35 @@
       </c>
       <c r="W17" s="34"/>
       <c r="AD17" s="34">
-        <f t="shared" ref="AD17:AE17" si="16">AD15-AD16</f>
+        <f t="shared" ref="AD17" si="31">AD15-AD16</f>
         <v>0</v>
       </c>
       <c r="AE17" s="34">
-        <f t="shared" ref="AE17:AI17" si="17">AE15-AE16</f>
+        <f t="shared" ref="AE17:AJ17" si="32">AE15-AE16</f>
         <v>0</v>
       </c>
       <c r="AF17" s="34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AG17" s="34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="32"/>
         <v>323</v>
       </c>
       <c r="AH17" s="34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="32"/>
         <v>892</v>
       </c>
       <c r="AI17" s="62">
-        <f t="shared" si="17"/>
+        <f t="shared" si="32"/>
         <v>434.38010499999962</v>
       </c>
-    </row>
-    <row r="18" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AJ17" s="34">
+        <f t="shared" si="32"/>
+        <v>728.07000933333359</v>
+      </c>
+    </row>
+    <row r="18" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>88</v>
       </c>
@@ -3276,86 +3570,109 @@
       <c r="D18" s="35"/>
       <c r="E18" s="35"/>
       <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
+      <c r="G18" s="28">
+        <f t="shared" ref="G18:I18" si="33">G17/G19</f>
+        <v>1.5302491103202847</v>
+      </c>
       <c r="H18" s="28">
-        <f t="shared" ref="H18:I18" si="18">H17/H19</f>
+        <f t="shared" si="33"/>
         <v>0.54151624548736466</v>
       </c>
       <c r="I18" s="28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="33"/>
         <v>1.1693171188026192</v>
       </c>
       <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
+      <c r="K18" s="28">
+        <f t="shared" ref="K18:V18" si="34">K17/K19</f>
+        <v>-1.0546500479386385</v>
+      </c>
       <c r="L18" s="28">
-        <f t="shared" ref="L18:V18" si="19">L17/L19</f>
+        <f t="shared" si="34"/>
         <v>0.43062200956937802</v>
       </c>
       <c r="M18" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>2.5383141762452106</v>
       </c>
-      <c r="N18" s="35"/>
+      <c r="N18" s="28">
+        <f t="shared" si="34"/>
+        <v>1.1792905081495686</v>
+      </c>
       <c r="O18" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>1.9498069498069499</v>
       </c>
       <c r="P18" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>4.1425818882466281</v>
       </c>
       <c r="Q18" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>1.5310077519379846</v>
       </c>
       <c r="R18" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>0.99512195121951219</v>
       </c>
       <c r="S18" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>1.3735691987513008</v>
       </c>
       <c r="T18" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>0.99893730074388953</v>
       </c>
       <c r="U18" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>1.0278372591006424</v>
       </c>
       <c r="V18" s="64">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>1.2032131156316928</v>
       </c>
       <c r="AG18" s="28">
-        <f t="shared" ref="AG18:AH18" si="20">AG17/AG19</f>
+        <f t="shared" ref="AG18:AJ18" si="35">AG17/AG19</f>
         <v>3.0968360498561842</v>
       </c>
       <c r="AH18" s="28">
-        <f t="shared" si="20"/>
+        <f t="shared" si="35"/>
         <v>8.7024390243902445</v>
       </c>
       <c r="AI18" s="65">
         <f>AI17/AI19</f>
         <v>4.6507505888650922</v>
       </c>
-    </row>
-    <row r="19" spans="2:35" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AJ18" s="28">
+        <f t="shared" si="35"/>
+        <v>7.7951821127765903</v>
+      </c>
+    </row>
+    <row r="19" spans="2:46" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="36" t="s">
         <v>4</v>
       </c>
+      <c r="G19" s="36">
+        <v>112.4</v>
+      </c>
       <c r="H19" s="36">
         <v>110.8</v>
       </c>
       <c r="I19" s="36">
         <v>106.9</v>
       </c>
+      <c r="K19" s="36">
+        <v>104.3</v>
+      </c>
       <c r="L19" s="36">
         <v>104.5</v>
       </c>
       <c r="M19" s="36">
         <v>104.4</v>
+      </c>
+      <c r="N19" s="36">
+        <f>AG19</f>
+        <v>104.3</v>
       </c>
       <c r="O19" s="36">
         <v>103.6</v>
@@ -3379,7 +3696,7 @@
       <c r="U19" s="36">
         <v>93.4</v>
       </c>
-      <c r="V19" s="79">
+      <c r="V19" s="67">
         <f>U19</f>
         <v>93.4</v>
       </c>
@@ -3389,29 +3706,53 @@
       <c r="AH19" s="36">
         <v>102.5</v>
       </c>
-      <c r="AI19" s="79">
+      <c r="AI19" s="67">
         <f>V19</f>
         <v>93.4</v>
       </c>
-    </row>
-    <row r="21" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AJ19" s="36">
+        <f>AI19</f>
+        <v>93.4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:46" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="K21" s="29">
+        <f t="shared" ref="K21" si="36">K6/G6-1</f>
+        <v>-0.43407122232916262</v>
+      </c>
       <c r="L21" s="29">
-        <f t="shared" ref="L21" si="21">L6/H6-1</f>
+        <f t="shared" ref="L21" si="37">L6/H6-1</f>
         <v>0.17080045095828633</v>
       </c>
       <c r="M21" s="29">
-        <f t="shared" ref="M21" si="22">M6/I6-1</f>
+        <f t="shared" ref="M21" si="38">M6/I6-1</f>
         <v>9.0062111801242128E-2</v>
       </c>
+      <c r="O21" s="29">
+        <f t="shared" ref="O21" si="39">O6/K6-1</f>
+        <v>0.83078231292517013</v>
+      </c>
+      <c r="P21" s="29">
+        <f t="shared" ref="P21" si="40">P6/L6-1</f>
+        <v>9.5329802599903646E-2</v>
+      </c>
+      <c r="Q21" s="29">
+        <f t="shared" ref="Q21" si="41">Q6/M6-1</f>
+        <v>3.9411206077872851E-2</v>
+      </c>
+      <c r="R21" s="29">
+        <f t="shared" ref="R21" si="42">R6/N6-1</f>
+        <v>6.9438099588853275E-2</v>
+      </c>
       <c r="S21" s="29">
-        <f t="shared" ref="S21" si="23">S6/O6-1</f>
+        <f t="shared" ref="S21" si="43">S6/O6-1</f>
         <v>1.021830004644686E-2</v>
       </c>
       <c r="T21" s="29">
-        <f t="shared" ref="T21" si="24">T6/P6-1</f>
+        <f t="shared" ref="T21" si="44">T6/P6-1</f>
         <v>-9.2307692307692313E-2</v>
       </c>
       <c r="U21" s="29">
@@ -3430,25 +3771,48 @@
         <f>AI6/AH6-1</f>
         <v>-2.9398303192677E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:35" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AJ21" s="29">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="22" spans="2:46" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="51" t="s">
         <v>125</v>
       </c>
+      <c r="K22" s="40">
+        <f t="shared" ref="K22:K23" si="45">K4/G4-1</f>
+        <v>-0.53697383390216147</v>
+      </c>
       <c r="L22" s="40">
-        <f t="shared" ref="L22:L23" si="25">L4/H4-1</f>
+        <f t="shared" ref="L22:L23" si="46">L4/H4-1</f>
         <v>-8.7442472057856713E-2</v>
       </c>
       <c r="M22" s="40">
-        <f t="shared" ref="M22:M23" si="26">M4/I4-1</f>
+        <f t="shared" ref="M22:M23" si="47">M4/I4-1</f>
         <v>1.2224938875305513E-2</v>
       </c>
+      <c r="O22" s="40">
+        <f t="shared" ref="O22:O23" si="48">O4/K4-1</f>
+        <v>0.99017199017199009</v>
+      </c>
+      <c r="P22" s="40">
+        <f t="shared" ref="P22:P23" si="49">P4/L4-1</f>
+        <v>0.30907780979827093</v>
+      </c>
+      <c r="Q22" s="40">
+        <f t="shared" ref="Q22:Q23" si="50">Q4/M4-1</f>
+        <v>6.0386473429951737E-2</v>
+      </c>
+      <c r="R22" s="40">
+        <f t="shared" ref="R22:R23" si="51">R4/N4-1</f>
+        <v>0.15544367526746372</v>
+      </c>
       <c r="S22" s="40">
-        <f t="shared" ref="S22:S23" si="27">S4/O4-1</f>
+        <f t="shared" ref="S22:S23" si="52">S4/O4-1</f>
         <v>9.6296296296296324E-2</v>
       </c>
       <c r="T22" s="40">
-        <f t="shared" ref="T22:T23" si="28">T4/P4-1</f>
+        <f t="shared" ref="T22:T23" si="53">T4/P4-1</f>
         <v>-5.5586130985140314E-2</v>
       </c>
       <c r="U22" s="40">
@@ -3462,24 +3826,44 @@
       </c>
       <c r="AI22" s="56"/>
     </row>
-    <row r="23" spans="2:35" s="40" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:46" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="51" t="s">
         <v>126</v>
       </c>
+      <c r="K23" s="40">
+        <f t="shared" si="45"/>
+        <v>0.13125000000000009</v>
+      </c>
       <c r="L23" s="40">
-        <f t="shared" si="25"/>
+        <f t="shared" si="46"/>
         <v>1.7233201581027666</v>
       </c>
       <c r="M23" s="40">
-        <f t="shared" si="26"/>
+        <f t="shared" si="47"/>
         <v>0.52027027027027017</v>
       </c>
+      <c r="O23" s="40">
+        <f t="shared" si="48"/>
+        <v>0.47237569060773477</v>
+      </c>
+      <c r="P23" s="40">
+        <f t="shared" si="49"/>
+        <v>-0.33526850507982586</v>
+      </c>
+      <c r="Q23" s="40">
+        <f t="shared" si="50"/>
+        <v>-3.7777777777777799E-2</v>
+      </c>
+      <c r="R23" s="40">
+        <f t="shared" si="51"/>
+        <v>-0.15833333333333333</v>
+      </c>
       <c r="S23" s="40">
-        <f t="shared" si="27"/>
+        <f t="shared" si="52"/>
         <v>-0.25140712945590993</v>
       </c>
       <c r="T23" s="40">
-        <f t="shared" si="28"/>
+        <f t="shared" si="53"/>
         <v>-0.23799126637554591</v>
       </c>
       <c r="U23" s="40">
@@ -3493,7 +3877,7 @@
       </c>
       <c r="AI23" s="56"/>
     </row>
-    <row r="24" spans="2:35" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:46" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="30" t="s">
         <v>90</v>
       </c>
@@ -3501,10 +3885,22 @@
         <f>I6/H6-1</f>
         <v>8.9064261555806157E-2</v>
       </c>
+      <c r="L24" s="30">
+        <f t="shared" ref="L24:M24" si="54">L6/K6-1</f>
+        <v>0.76615646258503411</v>
+      </c>
       <c r="M24" s="30">
         <f>M6/L6-1</f>
         <v>1.3962445835339343E-2</v>
       </c>
+      <c r="N24" s="30">
+        <f t="shared" ref="N24:O24" si="55">N6/M6-1</f>
+        <v>3.9411206077872851E-2</v>
+      </c>
+      <c r="O24" s="30">
+        <f t="shared" si="55"/>
+        <v>-1.6445865692096828E-2</v>
+      </c>
       <c r="P24" s="30">
         <f>P6/O6-1</f>
         <v>5.666511843938693E-2</v>
@@ -3514,15 +3910,15 @@
         <v>-3.7802197802197846E-2</v>
       </c>
       <c r="R24" s="30">
-        <f t="shared" ref="R24:T24" si="29">R6/Q6-1</f>
+        <f t="shared" ref="R24:T24" si="56">R6/Q6-1</f>
         <v>6.9438099588853275E-2</v>
       </c>
       <c r="S24" s="30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="56"/>
         <v>-7.0909867577958141E-2</v>
       </c>
       <c r="T24" s="30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="56"/>
         <v>-5.0574712643678188E-2</v>
       </c>
       <c r="U24" s="30">
@@ -3546,32 +3942,44 @@
       </c>
       <c r="AI24" s="56"/>
     </row>
-    <row r="26" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="G26" s="30">
+        <f t="shared" ref="G26:H26" si="57">G8/G6</f>
+        <v>0.33156881616939365</v>
+      </c>
       <c r="H26" s="30">
-        <f t="shared" ref="H26:I26" si="30">H8/H6</f>
+        <f t="shared" ref="H26:I26" si="58">H8/H6</f>
         <v>0.30101465614430667</v>
       </c>
       <c r="I26" s="30">
-        <f t="shared" si="30"/>
+        <f t="shared" si="58"/>
         <v>0.32091097308488614</v>
       </c>
+      <c r="K26" s="30">
+        <f t="shared" ref="K26:L26" si="59">K8/K6</f>
+        <v>0.23044217687074831</v>
+      </c>
       <c r="L26" s="30">
-        <f t="shared" ref="L26:M26" si="31">L8/L6</f>
+        <f t="shared" si="59"/>
         <v>0.2590274434280212</v>
       </c>
       <c r="M26" s="30">
-        <f t="shared" ref="M26:O26" si="32">M8/M6</f>
+        <f t="shared" ref="M26:O26" si="60">M8/M6</f>
         <v>0.30864197530864196</v>
       </c>
+      <c r="N26" s="30">
+        <f t="shared" ref="N26" si="61">N8/N6</f>
+        <v>0.33074463225216993</v>
+      </c>
       <c r="O26" s="30">
-        <f t="shared" si="32"/>
+        <f t="shared" si="60"/>
         <v>0.34788666976312121</v>
       </c>
       <c r="P26" s="30">
-        <f t="shared" ref="P26" si="33">P8/P6</f>
+        <f t="shared" ref="P26" si="62">P8/P6</f>
         <v>0.35076923076923078</v>
       </c>
       <c r="Q26" s="30">
@@ -3579,15 +3987,15 @@
         <v>0.34719049794426676</v>
       </c>
       <c r="R26" s="30">
-        <f t="shared" ref="R26" si="34">R8/R6</f>
+        <f t="shared" ref="R26" si="63">R8/R6</f>
         <v>0.33020076890217853</v>
       </c>
       <c r="S26" s="30">
-        <f t="shared" ref="S26" si="35">S8/S6</f>
+        <f t="shared" ref="S26" si="64">S8/S6</f>
         <v>0.34022988505747126</v>
       </c>
       <c r="T26" s="30">
-        <f t="shared" ref="T26" si="36">T8/T6</f>
+        <f t="shared" ref="T26" si="65">T8/T6</f>
         <v>0.31670702179176757</v>
       </c>
       <c r="U26" s="30">
@@ -3609,33 +4017,78 @@
         <f>AI8/AI6</f>
         <v>0.32435210157970706</v>
       </c>
-    </row>
-    <row r="27" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AJ26" s="30">
+        <v>0.34</v>
+      </c>
+      <c r="AK26" s="30">
+        <v>0.35</v>
+      </c>
+      <c r="AL26" s="30">
+        <v>0.35</v>
+      </c>
+      <c r="AM26" s="30">
+        <v>0.35</v>
+      </c>
+      <c r="AN26" s="30">
+        <v>0.35</v>
+      </c>
+      <c r="AO26" s="30">
+        <v>0.35</v>
+      </c>
+      <c r="AP26" s="30">
+        <v>0.35</v>
+      </c>
+      <c r="AQ26" s="30">
+        <v>0.35</v>
+      </c>
+      <c r="AR26" s="30">
+        <v>0.35</v>
+      </c>
+      <c r="AS26" s="30">
+        <v>0.35</v>
+      </c>
+      <c r="AT26" s="30">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="27" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="G27" s="30">
+        <f t="shared" ref="G27:H27" si="66">G12/G6</f>
+        <v>0.109720885466795</v>
+      </c>
       <c r="H27" s="30">
-        <f t="shared" ref="H27:I27" si="37">H12/H6</f>
+        <f t="shared" ref="H27:I27" si="67">H12/H6</f>
         <v>4.5659526493799327E-2</v>
       </c>
       <c r="I27" s="30">
-        <f t="shared" si="37"/>
+        <f t="shared" si="67"/>
         <v>8.4886128364389232E-2</v>
       </c>
+      <c r="K27" s="30">
+        <f t="shared" ref="K27:L27" si="68">K12/K6</f>
+        <v>-8.9285714285714288E-2</v>
+      </c>
       <c r="L27" s="30">
-        <f t="shared" ref="L27:M27" si="38">L12/L6</f>
+        <f t="shared" si="68"/>
         <v>3.3220991815117958E-2</v>
       </c>
       <c r="M27" s="30">
-        <f t="shared" ref="M27:O27" si="39">M12/M6</f>
+        <f t="shared" ref="M27:O27" si="69">M12/M6</f>
         <v>8.4520417853751181E-2</v>
       </c>
+      <c r="N27" s="30">
+        <f t="shared" ref="N27" si="70">N12/N6</f>
+        <v>7.3549566011877565E-2</v>
+      </c>
       <c r="O27" s="30">
-        <f t="shared" si="39"/>
+        <f t="shared" si="69"/>
         <v>0.13098002786809104</v>
       </c>
       <c r="P27" s="30">
-        <f t="shared" ref="P27" si="40">P12/P6</f>
+        <f t="shared" ref="P27" si="71">P12/P6</f>
         <v>0.11604395604395605</v>
       </c>
       <c r="Q27" s="30">
@@ -3643,15 +4096,15 @@
         <v>8.9538602101416176E-2</v>
       </c>
       <c r="R27" s="30">
-        <f t="shared" ref="R27" si="41">R12/R6</f>
+        <f t="shared" ref="R27" si="72">R12/R6</f>
         <v>5.0405809483126868E-2</v>
       </c>
       <c r="S27" s="30">
-        <f t="shared" ref="S27" si="42">S12/S6</f>
+        <f t="shared" ref="S27" si="73">S12/S6</f>
         <v>9.9770114942528743E-2</v>
       </c>
       <c r="T27" s="30">
-        <f t="shared" ref="T27" si="43">T12/T6</f>
+        <f t="shared" ref="T27" si="74">T12/T6</f>
         <v>6.7312348668280869E-2</v>
       </c>
       <c r="U27" s="30">
@@ -3674,33 +4127,49 @@
         <f>AI12/AI6</f>
         <v>7.8523172295607027E-2</v>
       </c>
-    </row>
-    <row r="28" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AJ27" s="30">
+        <f>AJ12/AJ6</f>
+        <v>9.5413081165296662E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="G28" s="30">
+        <f t="shared" ref="G28:H28" si="75">G17/G6</f>
+        <v>8.2771896053897981E-2</v>
+      </c>
       <c r="H28" s="30">
-        <f t="shared" ref="H28:I28" si="44">H17/H6</f>
+        <f t="shared" ref="H28:I28" si="76">H17/H6</f>
         <v>3.3821871476888386E-2</v>
       </c>
       <c r="I28" s="30">
-        <f t="shared" si="44"/>
+        <f t="shared" si="76"/>
         <v>6.4699792960662528E-2</v>
       </c>
+      <c r="K28" s="30">
+        <f t="shared" ref="K28:L28" si="77">K17/K6</f>
+        <v>-9.3537414965986401E-2</v>
+      </c>
       <c r="L28" s="30">
-        <f t="shared" ref="L28:M28" si="45">L17/L6</f>
+        <f t="shared" si="77"/>
         <v>2.1665864227250843E-2</v>
       </c>
       <c r="M28" s="30">
-        <f t="shared" ref="M28:O28" si="46">M17/M6</f>
+        <f t="shared" ref="M28:O28" si="78">M17/M6</f>
         <v>0.12583095916429249</v>
       </c>
+      <c r="N28" s="30">
+        <f t="shared" ref="N28" si="79">N17/N6</f>
+        <v>5.6190041114664233E-2</v>
+      </c>
       <c r="O28" s="30">
-        <f t="shared" si="46"/>
+        <f t="shared" si="78"/>
         <v>9.3822573153738972E-2</v>
       </c>
       <c r="P28" s="30">
-        <f t="shared" ref="P28" si="47">P17/P6</f>
+        <f t="shared" ref="P28" si="80">P17/P6</f>
         <v>0.18901098901098901</v>
       </c>
       <c r="Q28" s="30">
@@ -3708,15 +4177,15 @@
         <v>7.2179077204202829E-2</v>
       </c>
       <c r="R28" s="30">
-        <f t="shared" ref="R28" si="48">R17/R6</f>
+        <f t="shared" ref="R28" si="81">R17/R6</f>
         <v>4.3571123451516446E-2</v>
       </c>
       <c r="S28" s="30">
-        <f t="shared" ref="S28" si="49">S17/S6</f>
+        <f t="shared" ref="S28" si="82">S17/S6</f>
         <v>6.0689655172413794E-2</v>
       </c>
       <c r="T28" s="30">
-        <f t="shared" ref="T28" si="50">T17/T6</f>
+        <f t="shared" ref="T28" si="83">T17/T6</f>
         <v>4.5520581113801452E-2</v>
       </c>
       <c r="U28" s="30">
@@ -3739,33 +4208,49 @@
         <f>AI17/AI6</f>
         <v>4.9959469903906387E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AJ28" s="30">
+        <f>AJ17/AJ6</f>
+        <v>8.0517021003337338E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="G29" s="30">
+        <f t="shared" ref="G29:H29" si="84">G16/G15</f>
+        <v>0.26495726495726496</v>
+      </c>
       <c r="H29" s="30">
-        <f t="shared" ref="H29:I29" si="51">H16/H15</f>
+        <f t="shared" ref="H29:I29" si="85">H16/H15</f>
         <v>0.29411764705882354</v>
       </c>
       <c r="I29" s="30">
-        <f t="shared" si="51"/>
+        <f t="shared" si="85"/>
         <v>0.26900584795321636</v>
       </c>
+      <c r="K29" s="30">
+        <f t="shared" ref="K29:L29" si="86">K16/K15</f>
+        <v>-4.7619047619047616E-2</v>
+      </c>
       <c r="L29" s="30">
-        <f t="shared" ref="L29:M29" si="52">L16/L15</f>
+        <f t="shared" si="86"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="M29" s="30">
-        <f t="shared" ref="M29:O29" si="53">M16/M15</f>
+        <f t="shared" ref="M29:O29" si="87">M16/M15</f>
         <v>0.28184281842818426</v>
       </c>
+      <c r="N29" s="30">
+        <f t="shared" ref="N29" si="88">N16/N15</f>
+        <v>0.23125000000000001</v>
+      </c>
       <c r="O29" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="87"/>
         <v>0.28873239436619719</v>
       </c>
       <c r="P29" s="30">
-        <f t="shared" ref="P29" si="54">P16/P15</f>
+        <f t="shared" ref="P29" si="89">P16/P15</f>
         <v>0.26746166950596251</v>
       </c>
       <c r="Q29" s="30">
@@ -3773,15 +4258,15 @@
         <v>0.28828828828828829</v>
       </c>
       <c r="R29" s="30">
-        <f t="shared" ref="R29" si="55">R16/R15</f>
+        <f t="shared" ref="R29" si="90">R16/R15</f>
         <v>0.30612244897959184</v>
       </c>
       <c r="S29" s="30">
-        <f t="shared" ref="S29" si="56">S16/S15</f>
+        <f t="shared" ref="S29" si="91">S16/S15</f>
         <v>0.30526315789473685</v>
       </c>
       <c r="T29" s="30">
-        <f t="shared" ref="T29" si="57">T16/T15</f>
+        <f t="shared" ref="T29" si="92">T16/T15</f>
         <v>0.34265734265734266</v>
       </c>
       <c r="U29" s="30">
@@ -3803,30 +4288,63 @@
         <f>AI16/AI15</f>
         <v>0.32521539648129721</v>
       </c>
-    </row>
-    <row r="30" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AJ29" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="AK29" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="AL29" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="AM29" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="AN29" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="AO29" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="AP29" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="AQ29" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="AR29" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="AS29" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="AT29" s="30">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:46" x14ac:dyDescent="0.2">
       <c r="Q30" s="30"/>
       <c r="U30" s="30"/>
     </row>
-    <row r="31" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I31" s="78"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="78"/>
-      <c r="L31" s="78"/>
-      <c r="M31" s="78"/>
-      <c r="N31" s="78"/>
-      <c r="O31" s="78"/>
-      <c r="P31" s="78"/>
-      <c r="Q31" s="78"/>
-      <c r="R31" s="78"/>
-      <c r="S31" s="78"/>
-      <c r="T31" s="78"/>
-      <c r="U31" s="78"/>
-    </row>
-    <row r="32" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="I31" s="66"/>
+      <c r="J31" s="66"/>
+      <c r="K31" s="66"/>
+      <c r="L31" s="66"/>
+      <c r="M31" s="66"/>
+      <c r="N31" s="66"/>
+      <c r="O31" s="66"/>
+      <c r="P31" s="66"/>
+      <c r="Q31" s="66"/>
+      <c r="R31" s="66"/>
+      <c r="S31" s="66"/>
+      <c r="T31" s="66"/>
+      <c r="U31" s="66"/>
+    </row>
+    <row r="32" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B32" s="31" t="s">
         <v>127</v>
       </c>
@@ -3837,11 +4355,21 @@
       <c r="B33" s="35" t="s">
         <v>128</v>
       </c>
+      <c r="G33" s="35">
+        <v>3129</v>
+      </c>
       <c r="I33" s="35">
         <v>3160</v>
       </c>
+      <c r="K33" s="35">
+        <v>3113</v>
+      </c>
       <c r="M33" s="35">
         <v>3032</v>
+      </c>
+      <c r="N33" s="35">
+        <f>AG33</f>
+        <v>2998</v>
       </c>
       <c r="O33" s="35">
         <v>2952</v>
@@ -3877,9 +4405,33 @@
       <c r="B34" s="47" t="s">
         <v>129</v>
       </c>
+      <c r="K34" s="48">
+        <f>K33-G33</f>
+        <v>-16</v>
+      </c>
       <c r="M34" s="48">
         <f>M33-I33</f>
         <v>-128</v>
+      </c>
+      <c r="N34" s="48">
+        <f t="shared" ref="N34:R34" si="93">N33-J33</f>
+        <v>2998</v>
+      </c>
+      <c r="O34" s="48">
+        <f t="shared" si="93"/>
+        <v>-161</v>
+      </c>
+      <c r="P34" s="48">
+        <f t="shared" si="93"/>
+        <v>2911</v>
+      </c>
+      <c r="Q34" s="48">
+        <f t="shared" si="93"/>
+        <v>-76</v>
+      </c>
+      <c r="R34" s="48">
+        <f t="shared" si="93"/>
+        <v>-140</v>
       </c>
       <c r="S34" s="48">
         <f>S33-O33</f>
@@ -3904,24 +4456,32 @@
       <c r="B35" s="41" t="s">
         <v>131</v>
       </c>
+      <c r="N35" s="42">
+        <f t="shared" ref="N35" si="94">N33-M33</f>
+        <v>-34</v>
+      </c>
+      <c r="O35" s="42">
+        <f t="shared" ref="O35" si="95">O33-N33</f>
+        <v>-46</v>
+      </c>
       <c r="P35" s="42">
-        <f t="shared" ref="P35:T35" si="58">P33-O33</f>
+        <f t="shared" ref="P35:T35" si="96">P33-O33</f>
         <v>-41</v>
       </c>
       <c r="Q35" s="42">
-        <f t="shared" si="58"/>
+        <f t="shared" si="96"/>
         <v>45</v>
       </c>
       <c r="R35" s="42">
-        <f t="shared" si="58"/>
+        <f t="shared" si="96"/>
         <v>-98</v>
       </c>
       <c r="S35" s="42">
-        <f t="shared" si="58"/>
+        <f t="shared" si="96"/>
         <v>-43</v>
       </c>
       <c r="T35" s="42">
-        <f t="shared" si="58"/>
+        <f t="shared" si="96"/>
         <v>-16</v>
       </c>
       <c r="U35" s="42">
@@ -3947,40 +4507,52 @@
       <c r="B36" s="43" t="s">
         <v>130</v>
       </c>
+      <c r="G36" s="44">
+        <f t="shared" ref="G36:K36" si="97">G4/G33</f>
+        <v>0.5618408437200384</v>
+      </c>
       <c r="I36" s="44">
-        <f t="shared" ref="I36" si="59">I4/I33</f>
+        <f t="shared" si="97"/>
         <v>0.51772151898734176</v>
       </c>
+      <c r="K36" s="44">
+        <f t="shared" si="97"/>
+        <v>0.26148409893992935</v>
+      </c>
       <c r="M36" s="44">
-        <f t="shared" ref="M36:U36" si="60">M4/M33</f>
+        <f t="shared" ref="M36:U36" si="98">M4/M33</f>
         <v>0.54617414248021112</v>
       </c>
+      <c r="N36" s="44">
+        <f t="shared" si="98"/>
+        <v>0.53002001334222815</v>
+      </c>
       <c r="O36" s="44">
-        <f t="shared" si="60"/>
+        <f t="shared" si="98"/>
         <v>0.54878048780487809</v>
       </c>
       <c r="P36" s="44">
-        <f t="shared" si="60"/>
+        <f t="shared" si="98"/>
         <v>0.62418412916523536</v>
       </c>
       <c r="Q36" s="44">
-        <f t="shared" si="60"/>
+        <f t="shared" si="98"/>
         <v>0.59404600811907982</v>
       </c>
       <c r="R36" s="44">
-        <f t="shared" si="60"/>
+        <f t="shared" si="98"/>
         <v>0.64240727781665496</v>
       </c>
       <c r="S36" s="44">
-        <f t="shared" si="60"/>
+        <f t="shared" si="98"/>
         <v>0.63090586145648309</v>
       </c>
       <c r="T36" s="44">
-        <f t="shared" si="60"/>
+        <f t="shared" si="98"/>
         <v>0.61307609860664525</v>
       </c>
       <c r="U36" s="44">
-        <f t="shared" si="60"/>
+        <f t="shared" si="98"/>
         <v>0.65068002863278451</v>
       </c>
       <c r="V36" s="60"/>
@@ -4046,6 +4618,10 @@
         <v>351</v>
       </c>
       <c r="V41" s="55"/>
+      <c r="AH41" s="34">
+        <f>R41</f>
+        <v>804</v>
+      </c>
       <c r="AI41" s="55"/>
     </row>
     <row r="42" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4090,6 +4666,10 @@
         <v>1685</v>
       </c>
       <c r="V42" s="55"/>
+      <c r="AH42" s="34">
+        <f>R42</f>
+        <v>1266</v>
+      </c>
       <c r="AI42" s="55"/>
     </row>
     <row r="43" spans="2:35" x14ac:dyDescent="0.2">
@@ -4133,69 +4713,73 @@
       <c r="U43" s="35">
         <v>302</v>
       </c>
+      <c r="AH43" s="35">
+        <f>R43</f>
+        <v>293</v>
+      </c>
     </row>
     <row r="44" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C44" s="35">
-        <f t="shared" ref="C44:T44" si="61">SUM(C41:C43)</f>
+        <f t="shared" ref="C44:T44" si="99">SUM(C41:C43)</f>
         <v>0</v>
       </c>
       <c r="D44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="E44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="F44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="G44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="H44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="I44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>2347</v>
       </c>
       <c r="J44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="L44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="M44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>2823</v>
       </c>
       <c r="N44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="O44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>3267</v>
       </c>
       <c r="P44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>3178</v>
       </c>
       <c r="Q44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>2893</v>
       </c>
       <c r="R44" s="35">
@@ -4203,16 +4787,20 @@
         <v>2363</v>
       </c>
       <c r="S44" s="35">
-        <f t="shared" ref="S44" si="62">SUM(S41:S43)</f>
+        <f t="shared" ref="S44" si="100">SUM(S41:S43)</f>
         <v>2233</v>
       </c>
       <c r="T44" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="99"/>
         <v>2315</v>
       </c>
       <c r="U44" s="35">
         <f>SUM(U41:U43)</f>
         <v>2338</v>
+      </c>
+      <c r="AH44" s="35">
+        <f>SUM(AH41:AH43)</f>
+        <v>2363</v>
       </c>
     </row>
     <row r="45" spans="2:35" x14ac:dyDescent="0.2">
@@ -4256,6 +4844,10 @@
       <c r="U45" s="35">
         <v>897</v>
       </c>
+      <c r="AH45" s="35">
+        <f t="shared" ref="AH45:AH50" si="101">R45</f>
+        <v>917</v>
+      </c>
     </row>
     <row r="46" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
@@ -4298,6 +4890,10 @@
       <c r="U46" s="35">
         <v>2449</v>
       </c>
+      <c r="AH46" s="35">
+        <f t="shared" si="101"/>
+        <v>2616</v>
+      </c>
     </row>
     <row r="47" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
@@ -4339,6 +4935,10 @@
       </c>
       <c r="U47" s="35">
         <v>65</v>
+      </c>
+      <c r="AH47" s="35">
+        <f t="shared" si="101"/>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="2:35" x14ac:dyDescent="0.2">
@@ -4391,6 +4991,10 @@
         <f>764+424</f>
         <v>1188</v>
       </c>
+      <c r="AH48" s="35">
+        <f t="shared" si="101"/>
+        <v>1251</v>
+      </c>
     </row>
     <row r="49" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
@@ -4433,6 +5037,10 @@
       <c r="U49" s="35">
         <v>722</v>
       </c>
+      <c r="AH49" s="35">
+        <f t="shared" si="101"/>
+        <v>781</v>
+      </c>
     </row>
     <row r="50" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
@@ -4475,69 +5083,73 @@
       <c r="U50" s="35">
         <v>103</v>
       </c>
+      <c r="AH50" s="35">
+        <f t="shared" si="101"/>
+        <v>121</v>
+      </c>
     </row>
     <row r="51" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C51" s="35">
-        <f t="shared" ref="C51:T51" si="63">SUM(C45:C50)+C44</f>
+        <f t="shared" ref="C51:T51" si="102">SUM(C45:C50)+C44</f>
         <v>0</v>
       </c>
       <c r="D51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>0</v>
       </c>
       <c r="E51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>0</v>
       </c>
       <c r="F51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>0</v>
       </c>
       <c r="G51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>0</v>
       </c>
       <c r="H51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>0</v>
       </c>
       <c r="I51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>6621</v>
       </c>
       <c r="J51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>0</v>
       </c>
       <c r="K51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>0</v>
       </c>
       <c r="L51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>0</v>
       </c>
       <c r="M51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>7018</v>
       </c>
       <c r="N51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>0</v>
       </c>
       <c r="O51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>7442</v>
       </c>
       <c r="P51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>7585</v>
       </c>
       <c r="Q51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>8211</v>
       </c>
       <c r="R51" s="35">
@@ -4545,16 +5157,20 @@
         <v>8135</v>
       </c>
       <c r="S51" s="35">
-        <f t="shared" ref="S51" si="64">SUM(S45:S50)+S44</f>
+        <f t="shared" ref="S51" si="103">SUM(S45:S50)+S44</f>
         <v>7878</v>
       </c>
       <c r="T51" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="102"/>
         <v>7868</v>
       </c>
       <c r="U51" s="35">
         <f>SUM(U45:U50)+U44</f>
         <v>7762</v>
+      </c>
+      <c r="AH51" s="35">
+        <f>SUM(AH45:AH50)+AH44</f>
+        <v>8135</v>
       </c>
     </row>
     <row r="53" spans="2:35" x14ac:dyDescent="0.2">
@@ -4598,6 +5214,10 @@
       <c r="U53" s="35">
         <v>522</v>
       </c>
+      <c r="AH53" s="35">
+        <f t="shared" ref="AH53:AH54" si="104">R53</f>
+        <v>596</v>
+      </c>
     </row>
     <row r="54" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
@@ -4640,6 +5260,10 @@
       <c r="U54" s="35">
         <v>455</v>
       </c>
+      <c r="AH54" s="35">
+        <f t="shared" si="104"/>
+        <v>561</v>
+      </c>
     </row>
     <row r="55" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
@@ -4683,6 +5307,10 @@
         <v>6</v>
       </c>
       <c r="V55" s="55"/>
+      <c r="AH55" s="34">
+        <f>R55</f>
+        <v>6</v>
+      </c>
       <c r="AI55" s="55"/>
     </row>
     <row r="56" spans="2:35" x14ac:dyDescent="0.2">
@@ -4726,69 +5354,73 @@
       <c r="U56" s="35">
         <v>539</v>
       </c>
+      <c r="AH56" s="35">
+        <f>R56</f>
+        <v>572</v>
+      </c>
     </row>
     <row r="57" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C57" s="35">
-        <f t="shared" ref="C57:T57" si="65">SUM(C53:C56)</f>
+        <f t="shared" ref="C57:T57" si="105">SUM(C53:C56)</f>
         <v>0</v>
       </c>
       <c r="D57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>0</v>
       </c>
       <c r="E57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>0</v>
       </c>
       <c r="F57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>0</v>
       </c>
       <c r="G57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>0</v>
       </c>
       <c r="H57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>0</v>
       </c>
       <c r="I57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>1237</v>
       </c>
       <c r="J57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>0</v>
       </c>
       <c r="K57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>0</v>
       </c>
       <c r="L57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>0</v>
       </c>
       <c r="M57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>1542</v>
       </c>
       <c r="N57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>0</v>
       </c>
       <c r="O57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>1913</v>
       </c>
       <c r="P57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>1681</v>
       </c>
       <c r="Q57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>1757</v>
       </c>
       <c r="R57" s="35">
@@ -4796,16 +5428,20 @@
         <v>1735</v>
       </c>
       <c r="S57" s="35">
-        <f t="shared" ref="S57" si="66">SUM(S53:S56)</f>
+        <f t="shared" ref="S57" si="106">SUM(S53:S56)</f>
         <v>1556</v>
       </c>
       <c r="T57" s="35">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>1585</v>
       </c>
       <c r="U57" s="35">
         <f>SUM(U53:U56)</f>
         <v>1522</v>
+      </c>
+      <c r="AH57" s="35">
+        <f t="shared" ref="AH57" si="107">SUM(AH53:AH56)</f>
+        <v>1735</v>
       </c>
     </row>
     <row r="58" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4850,6 +5486,10 @@
         <v>448</v>
       </c>
       <c r="V58" s="55"/>
+      <c r="AH58" s="34">
+        <f>R58</f>
+        <v>451</v>
+      </c>
       <c r="AI58" s="55"/>
     </row>
     <row r="59" spans="2:35" x14ac:dyDescent="0.2">
@@ -4893,6 +5533,10 @@
       <c r="U59" s="35">
         <v>2212</v>
       </c>
+      <c r="AH59" s="35">
+        <f t="shared" ref="AH59:AH60" si="108">R59</f>
+        <v>2363</v>
+      </c>
     </row>
     <row r="60" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
@@ -4935,69 +5579,73 @@
       <c r="U60" s="35">
         <v>321</v>
       </c>
+      <c r="AH60" s="35">
+        <f t="shared" si="108"/>
+        <v>343</v>
+      </c>
     </row>
     <row r="61" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C61" s="35">
-        <f t="shared" ref="C61:T61" si="67">SUM(C58:C60)+C57</f>
+        <f t="shared" ref="C61:T61" si="109">SUM(C58:C60)+C57</f>
         <v>0</v>
       </c>
       <c r="D61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="E61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="F61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="G61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="H61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="I61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>3654</v>
       </c>
       <c r="J61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="K61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="L61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="M61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>4366</v>
       </c>
       <c r="N61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="O61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>4512</v>
       </c>
       <c r="P61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>4244</v>
       </c>
       <c r="Q61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>4869</v>
       </c>
       <c r="R61" s="35">
@@ -5005,17 +5653,21 @@
         <v>4892</v>
       </c>
       <c r="S61" s="35">
-        <f t="shared" ref="S61" si="68">SUM(S58:S60)+S57</f>
+        <f t="shared" ref="S61" si="110">SUM(S58:S60)+S57</f>
         <v>4663</v>
       </c>
       <c r="T61" s="35">
-        <f t="shared" si="67"/>
+        <f t="shared" si="109"/>
         <v>4651</v>
       </c>
       <c r="U61" s="35">
         <f>SUM(U58:U60)+U57</f>
         <v>4503</v>
       </c>
+      <c r="AH61" s="35">
+        <f t="shared" ref="AH61" si="111">SUM(AH58:AH60)+AH57</f>
+        <v>4892</v>
+      </c>
     </row>
     <row r="63" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
@@ -5048,69 +5700,73 @@
       <c r="U63" s="35">
         <v>3259</v>
       </c>
+      <c r="AH63" s="35">
+        <f>R63</f>
+        <v>3243</v>
+      </c>
     </row>
     <row r="64" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
         <v>116</v>
       </c>
       <c r="C64" s="35">
-        <f t="shared" ref="C64:T64" si="69">C63+C61</f>
+        <f t="shared" ref="C64:T64" si="112">C63+C61</f>
         <v>0</v>
       </c>
       <c r="D64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="E64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="F64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="G64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="H64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="I64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>6081</v>
       </c>
       <c r="J64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="K64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="L64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="M64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>7018</v>
       </c>
       <c r="N64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
       <c r="O64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>7442</v>
       </c>
       <c r="P64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>7585</v>
       </c>
       <c r="Q64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>8211</v>
       </c>
       <c r="R64" s="35">
@@ -5118,36 +5774,40 @@
         <v>8135</v>
       </c>
       <c r="S64" s="35">
-        <f t="shared" ref="S64" si="70">S63+S61</f>
+        <f t="shared" ref="S64" si="113">S63+S61</f>
         <v>7878</v>
       </c>
       <c r="T64" s="35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="112"/>
         <v>7868</v>
       </c>
       <c r="U64" s="35">
         <f>U63+U61</f>
         <v>7762</v>
       </c>
+      <c r="AH64" s="35">
+        <f t="shared" ref="AH64" si="114">AH63+AH61</f>
+        <v>8135</v>
+      </c>
     </row>
     <row r="66" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
         <v>117</v>
       </c>
       <c r="I66" s="35">
-        <f t="shared" ref="I66" si="71">I51-I61</f>
+        <f t="shared" ref="I66" si="115">I51-I61</f>
         <v>2967</v>
       </c>
       <c r="M66" s="35">
-        <f t="shared" ref="M66:O66" si="72">M51-M61</f>
+        <f t="shared" ref="M66:O66" si="116">M51-M61</f>
         <v>2652</v>
       </c>
       <c r="O66" s="35">
-        <f t="shared" si="72"/>
+        <f t="shared" si="116"/>
         <v>2930</v>
       </c>
       <c r="P66" s="35">
-        <f t="shared" ref="P66" si="73">P51-P61</f>
+        <f t="shared" ref="P66" si="117">P51-P61</f>
         <v>3341</v>
       </c>
       <c r="Q66" s="35">
@@ -5159,36 +5819,40 @@
         <v>3243</v>
       </c>
       <c r="S66" s="35">
-        <f t="shared" ref="S66" si="74">S51-S61</f>
+        <f t="shared" ref="S66" si="118">S51-S61</f>
         <v>3215</v>
       </c>
       <c r="T66" s="35">
-        <f t="shared" ref="T66" si="75">T51-T61</f>
+        <f t="shared" ref="T66" si="119">T51-T61</f>
         <v>3217</v>
       </c>
       <c r="U66" s="35">
         <f>U51-U61</f>
         <v>3259</v>
       </c>
+      <c r="AH66" s="35">
+        <f>AH51-AH61</f>
+        <v>3243</v>
+      </c>
     </row>
     <row r="67" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
         <v>118</v>
       </c>
       <c r="I67" s="1">
-        <f t="shared" ref="I67" si="76">I66/I19</f>
+        <f t="shared" ref="I67" si="120">I66/I19</f>
         <v>27.754911131898968</v>
       </c>
       <c r="M67" s="1">
-        <f t="shared" ref="M67:O67" si="77">M66/M19</f>
+        <f t="shared" ref="M67:O67" si="121">M66/M19</f>
         <v>25.402298850574713</v>
       </c>
       <c r="O67" s="1">
-        <f t="shared" si="77"/>
+        <f t="shared" si="121"/>
         <v>28.281853281853284</v>
       </c>
       <c r="P67" s="1">
-        <f t="shared" ref="P67" si="78">P66/P19</f>
+        <f t="shared" ref="P67" si="122">P66/P19</f>
         <v>32.186897880539497</v>
       </c>
       <c r="Q67" s="1">
@@ -5196,84 +5860,88 @@
         <v>32.383720930232556</v>
       </c>
       <c r="R67" s="1">
-        <f t="shared" ref="R67:S67" si="79">R66/R19</f>
+        <f t="shared" ref="R67:S67" si="123">R66/R19</f>
         <v>31.639024390243904</v>
       </c>
       <c r="S67" s="1">
-        <f t="shared" si="79"/>
+        <f t="shared" si="123"/>
         <v>33.454734651404792</v>
       </c>
       <c r="T67" s="1">
-        <f t="shared" ref="T67" si="80">T66/T19</f>
+        <f t="shared" ref="T67" si="124">T66/T19</f>
         <v>34.187035069075456</v>
       </c>
       <c r="U67" s="1">
         <f>U66/U19</f>
         <v>34.892933618843678</v>
       </c>
+      <c r="AH67" s="1">
+        <f>AH66/AH19</f>
+        <v>31.639024390243904</v>
+      </c>
     </row>
     <row r="69" spans="2:35" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B69" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C69" s="37">
-        <f t="shared" ref="C69:T69" si="81">C41</f>
+        <f t="shared" ref="C69:T69" si="125">C41</f>
         <v>0</v>
       </c>
       <c r="D69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>0</v>
       </c>
       <c r="E69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>0</v>
       </c>
       <c r="F69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>0</v>
       </c>
       <c r="G69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>0</v>
       </c>
       <c r="H69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>0</v>
       </c>
       <c r="I69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>744</v>
       </c>
       <c r="J69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>0</v>
       </c>
       <c r="K69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>0</v>
       </c>
       <c r="L69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>0</v>
       </c>
       <c r="M69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>1393</v>
       </c>
       <c r="N69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>0</v>
       </c>
       <c r="O69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>1963</v>
       </c>
       <c r="P69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>1845</v>
       </c>
       <c r="Q69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>1339</v>
       </c>
       <c r="R69" s="37">
@@ -5281,11 +5949,11 @@
         <v>804</v>
       </c>
       <c r="S69" s="37">
-        <f t="shared" ref="S69" si="82">S41</f>
+        <f t="shared" ref="S69" si="126">S41</f>
         <v>551</v>
       </c>
       <c r="T69" s="37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="125"/>
         <v>386</v>
       </c>
       <c r="U69" s="37">
@@ -5293,6 +5961,10 @@
         <v>351</v>
       </c>
       <c r="V69" s="54"/>
+      <c r="AH69" s="37">
+        <f>AH41</f>
+        <v>804</v>
+      </c>
       <c r="AI69" s="54"/>
     </row>
     <row r="70" spans="2:35" s="32" customFormat="1" x14ac:dyDescent="0.2">
@@ -5300,63 +5972,63 @@
         <v>7</v>
       </c>
       <c r="C70" s="37">
-        <f t="shared" ref="C70:T70" si="83">C55+C58</f>
+        <f t="shared" ref="C70:T70" si="127">C55+C58</f>
         <v>0</v>
       </c>
       <c r="D70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>0</v>
       </c>
       <c r="E70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>0</v>
       </c>
       <c r="F70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>0</v>
       </c>
       <c r="G70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>0</v>
       </c>
       <c r="H70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>0</v>
       </c>
       <c r="I70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>122</v>
       </c>
       <c r="J70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>0</v>
       </c>
       <c r="K70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>0</v>
       </c>
       <c r="L70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>0</v>
       </c>
       <c r="M70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>131</v>
       </c>
       <c r="N70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>0</v>
       </c>
       <c r="O70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>109</v>
       </c>
       <c r="P70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>112</v>
       </c>
       <c r="Q70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>560</v>
       </c>
       <c r="R70" s="37">
@@ -5364,11 +6036,11 @@
         <v>457</v>
       </c>
       <c r="S70" s="37">
-        <f t="shared" ref="S70" si="84">S55+S58</f>
+        <f t="shared" ref="S70" si="128">S55+S58</f>
         <v>456</v>
       </c>
       <c r="T70" s="37">
-        <f t="shared" si="83"/>
+        <f t="shared" si="127"/>
         <v>455</v>
       </c>
       <c r="U70" s="37">
@@ -5376,6 +6048,10 @@
         <v>454</v>
       </c>
       <c r="V70" s="54"/>
+      <c r="AH70" s="37">
+        <f>AH55+AH58</f>
+        <v>457</v>
+      </c>
       <c r="AI70" s="54"/>
     </row>
     <row r="71" spans="2:35" x14ac:dyDescent="0.2">
@@ -5383,63 +6059,63 @@
         <v>8</v>
       </c>
       <c r="C71" s="35">
-        <f t="shared" ref="C71:T71" si="85">C69-C70</f>
+        <f t="shared" ref="C71:T71" si="129">C69-C70</f>
         <v>0</v>
       </c>
       <c r="D71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>0</v>
       </c>
       <c r="E71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>0</v>
       </c>
       <c r="F71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>0</v>
       </c>
       <c r="G71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>0</v>
       </c>
       <c r="H71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>0</v>
       </c>
       <c r="I71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>622</v>
       </c>
       <c r="J71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>0</v>
       </c>
       <c r="K71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>0</v>
       </c>
       <c r="L71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>0</v>
       </c>
       <c r="M71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>1262</v>
       </c>
       <c r="N71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>0</v>
       </c>
       <c r="O71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>1854</v>
       </c>
       <c r="P71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>1733</v>
       </c>
       <c r="Q71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>779</v>
       </c>
       <c r="R71" s="35">
@@ -5447,32 +6123,36 @@
         <v>347</v>
       </c>
       <c r="S71" s="35">
-        <f t="shared" ref="S71" si="86">S69-S70</f>
+        <f t="shared" ref="S71" si="130">S69-S70</f>
         <v>95</v>
       </c>
       <c r="T71" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="129"/>
         <v>-69</v>
       </c>
       <c r="U71" s="35">
         <f>U69-U70</f>
         <v>-103</v>
       </c>
+      <c r="AH71" s="35">
+        <f>AH69-AH70</f>
+        <v>347</v>
+      </c>
     </row>
     <row r="73" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B73" s="2" t="s">
         <v>119</v>
       </c>
       <c r="M73" s="30">
-        <f t="shared" ref="M73" si="87">M42/I42-1</f>
+        <f t="shared" ref="M73" si="131">M42/I42-1</f>
         <v>-8.5122699386503076E-2</v>
       </c>
       <c r="Q73" s="30">
-        <f t="shared" ref="Q73:S73" si="88">Q42/M42-1</f>
+        <f t="shared" ref="Q73:S73" si="132">Q42/M42-1</f>
         <v>9.0528080469404859E-2</v>
       </c>
       <c r="S73" s="30">
-        <f t="shared" si="88"/>
+        <f t="shared" si="132"/>
         <v>0.37218413320274246</v>
       </c>
       <c r="T73" s="30">
@@ -5489,7 +6169,7 @@
         <v>122</v>
       </c>
       <c r="P74" s="30">
-        <f t="shared" ref="P74" si="89">P42/O42-1</f>
+        <f t="shared" ref="P74" si="133">P42/O42-1</f>
         <v>5.8765915768854038E-2</v>
       </c>
       <c r="Q74" s="30">
@@ -5501,11 +6181,11 @@
         <v>-2.6902382782475032E-2</v>
       </c>
       <c r="S74" s="30">
-        <f t="shared" ref="S74:T74" si="90">S42/R42-1</f>
+        <f t="shared" ref="S74:T74" si="134">S42/R42-1</f>
         <v>0.10663507109004744</v>
       </c>
       <c r="T74" s="30">
-        <f t="shared" si="90"/>
+        <f t="shared" si="134"/>
         <v>0.17344753747323338</v>
       </c>
       <c r="U74" s="30">
@@ -5520,21 +6200,25 @@
         <v>120</v>
       </c>
       <c r="R75" s="30">
-        <f t="shared" ref="R75:T75" si="91">R42/SUM(O6:R6)</f>
+        <f t="shared" ref="R75:T75" si="135">R42/SUM(O6:R6)</f>
         <v>0.14132618888144674</v>
       </c>
       <c r="S75" s="30">
-        <f t="shared" si="91"/>
+        <f t="shared" si="135"/>
         <v>0.15601336302895322</v>
       </c>
       <c r="T75" s="30">
-        <f t="shared" si="91"/>
+        <f t="shared" si="135"/>
         <v>0.18745724059293045</v>
       </c>
       <c r="U75" s="30">
         <f>U42/SUM(R6:U6)</f>
         <v>0.19248343614347727</v>
       </c>
+      <c r="AH75" s="30">
+        <f>AH42/AH6</f>
+        <v>0.14132618888144674</v>
+      </c>
     </row>
     <row r="77" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B77" s="28" t="s">
@@ -5561,17 +6245,21 @@
       <c r="U77" s="38">
         <v>31.1</v>
       </c>
+      <c r="AH77" s="1">
+        <f>R77</f>
+        <v>42.16</v>
+      </c>
     </row>
     <row r="78" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="s">
         <v>5</v>
       </c>
       <c r="O78" s="35">
-        <f t="shared" ref="O78" si="92">O77*O19</f>
+        <f t="shared" ref="O78" si="136">O77*O19</f>
         <v>6119.652</v>
       </c>
       <c r="P78" s="35">
-        <f t="shared" ref="P78" si="93">P77*P19</f>
+        <f t="shared" ref="P78" si="137">P77*P19</f>
         <v>5546.0339999999997</v>
       </c>
       <c r="Q78" s="35">
@@ -5579,32 +6267,36 @@
         <v>4635.7440000000006</v>
       </c>
       <c r="R78" s="35">
-        <f t="shared" ref="R78" si="94">R77*R19</f>
+        <f t="shared" ref="R78" si="138">R77*R19</f>
         <v>4321.3999999999996</v>
       </c>
       <c r="S78" s="35">
-        <f t="shared" ref="S78" si="95">S77*S19</f>
+        <f t="shared" ref="S78" si="139">S77*S19</f>
         <v>2710.02</v>
       </c>
       <c r="T78" s="35">
-        <f t="shared" ref="T78" si="96">T77*T19</f>
+        <f t="shared" ref="T78" si="140">T77*T19</f>
         <v>2610.3339999999998</v>
       </c>
       <c r="U78" s="35">
         <f>U77*U19</f>
         <v>2904.7400000000002</v>
       </c>
+      <c r="AH78" s="35">
+        <f>AH77*AH19</f>
+        <v>4321.3999999999996</v>
+      </c>
     </row>
     <row r="79" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
         <v>9</v>
       </c>
       <c r="O79" s="35">
-        <f t="shared" ref="O79" si="97">O78-O71</f>
+        <f t="shared" ref="O79" si="141">O78-O71</f>
         <v>4265.652</v>
       </c>
       <c r="P79" s="35">
-        <f t="shared" ref="P79" si="98">P78-P71</f>
+        <f t="shared" ref="P79" si="142">P78-P71</f>
         <v>3813.0339999999997</v>
       </c>
       <c r="Q79" s="35">
@@ -5612,32 +6304,36 @@
         <v>3856.7440000000006</v>
       </c>
       <c r="R79" s="35">
-        <f t="shared" ref="R79" si="99">R78-R71</f>
+        <f t="shared" ref="R79" si="143">R78-R71</f>
         <v>3974.3999999999996</v>
       </c>
       <c r="S79" s="35">
-        <f t="shared" ref="S79" si="100">S78-S71</f>
+        <f t="shared" ref="S79" si="144">S78-S71</f>
         <v>2615.02</v>
       </c>
       <c r="T79" s="35">
-        <f t="shared" ref="T79" si="101">T78-T71</f>
+        <f t="shared" ref="T79" si="145">T78-T71</f>
         <v>2679.3339999999998</v>
       </c>
       <c r="U79" s="35">
         <f>U78-U71</f>
         <v>3007.7400000000002</v>
       </c>
+      <c r="AH79" s="35">
+        <f>AH78-AH71</f>
+        <v>3974.3999999999996</v>
+      </c>
     </row>
     <row r="81" spans="2:35" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B81" s="33" t="s">
         <v>22</v>
       </c>
       <c r="O81" s="33">
-        <f t="shared" ref="O81" si="102">O77/O67</f>
+        <f t="shared" ref="O81" si="146">O77/O67</f>
         <v>2.0886184300341295</v>
       </c>
       <c r="P81" s="33">
-        <f t="shared" ref="P81" si="103">P77/P67</f>
+        <f t="shared" ref="P81" si="147">P77/P67</f>
         <v>1.6599922178988327</v>
       </c>
       <c r="Q81" s="33">
@@ -5645,15 +6341,15 @@
         <v>1.387116696588869</v>
       </c>
       <c r="R81" s="33">
-        <f t="shared" ref="R81" si="104">R77/R67</f>
+        <f t="shared" ref="R81" si="148">R77/R67</f>
         <v>1.3325316065371569</v>
       </c>
       <c r="S81" s="33">
-        <f t="shared" ref="S81" si="105">S77/S67</f>
+        <f t="shared" ref="S81" si="149">S77/S67</f>
         <v>0.84293001555209934</v>
       </c>
       <c r="T81" s="33">
-        <f t="shared" ref="T81" si="106">T77/T67</f>
+        <f t="shared" ref="T81" si="150">T77/T67</f>
         <v>0.81141871308672664</v>
       </c>
       <c r="U81" s="33">
@@ -5661,42 +6357,62 @@
         <v>0.8912979441546488</v>
       </c>
       <c r="V81" s="61"/>
+      <c r="AH81" s="33">
+        <f>AH77/AH67</f>
+        <v>1.3325316065371569</v>
+      </c>
       <c r="AI81" s="61"/>
     </row>
     <row r="82" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B82" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="AH82" s="33">
+        <f>AH78/AH6</f>
+        <v>0.4824067872292922</v>
+      </c>
     </row>
     <row r="83" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B83" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="AH83" s="33">
+        <f>AH79/AH6</f>
+        <v>0.44367046215673139</v>
+      </c>
     </row>
     <row r="84" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B84" s="1" t="s">
         <v>25</v>
       </c>
       <c r="R84" s="33">
-        <f t="shared" ref="R84:T84" si="107">R77/SUM(O18:R18)</f>
+        <f t="shared" ref="R84:T84" si="151">R77/SUM(O18:R18)</f>
         <v>4.8917919939957191</v>
       </c>
       <c r="S84" s="33">
-        <f t="shared" si="107"/>
+        <f t="shared" si="151"/>
         <v>3.5064679704443651</v>
       </c>
       <c r="T84" s="33">
-        <f t="shared" si="107"/>
+        <f t="shared" si="151"/>
         <v>5.662800594373258</v>
       </c>
       <c r="U84" s="33">
         <f>U77/SUM(R18:U18)</f>
         <v>7.0754732383764916</v>
       </c>
+      <c r="AH84" s="33">
+        <f>AH77/AH18</f>
+        <v>4.844618834080717</v>
+      </c>
     </row>
     <row r="85" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B85" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="AH85" s="33">
+        <f>AH79/AH17</f>
+        <v>4.4556053811659186</v>
       </c>
     </row>
     <row r="86" spans="2:35" x14ac:dyDescent="0.2">
@@ -5713,14 +6429,15 @@
     <hyperlink ref="AH1" r:id="rId5" xr:uid="{38A8ED3A-2717-4FEA-BB5C-B793AAB5C38B}"/>
     <hyperlink ref="M1" r:id="rId6" xr:uid="{43A5C21D-F886-4FCB-A94B-86147CFAE126}"/>
     <hyperlink ref="L1" r:id="rId7" xr:uid="{9446438F-F601-4E14-BBC3-368E3CAEABAA}"/>
+    <hyperlink ref="K1" r:id="rId8" xr:uid="{98932DF5-0820-4069-ACE8-E0B2BFF6C5E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId8"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId9"/>
   <ignoredErrors>
-    <ignoredError sqref="R6:R17 V12 AI8:AI15 AI16:AI19" formula="1"/>
+    <ignoredError sqref="R6:R17 V12 AI8:AI15 AI16:AI19 T44 T51:T68 AH59:AH64 AH57:AH58 AH44:AH56 AJ12 N6:N19" formula="1"/>
     <ignoredError sqref="AH8 AH15 AH12" formula="1" formulaRange="1"/>
     <ignoredError sqref="AH17" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId9"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update footwear retailer latest prices
</commit_message>
<xml_diff>
--- a/$FL.xlsx
+++ b/$FL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12355777-BC27-485C-846B-C95C62454C71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7C1B7C-A5E2-4F7B-9811-53D2F4ABD2DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{77D9C7A4-F0C3-486A-8AA0-E7E6A2714164}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="12225" xr2:uid="{77D9C7A4-F0C3-486A-8AA0-E7E6A2714164}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -812,6 +812,17 @@
     <xf numFmtId="16" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -824,10 +835,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -845,20 +853,12 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1345,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D13917F-DFCA-4AA6-ACFC-026B1E81207F}">
-  <dimension ref="A2:Q41"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1356,6 +1356,9 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="H1" s="29"/>
+    </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1367,31 +1370,31 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="74"/>
-      <c r="G5" s="72" t="s">
+      <c r="C5" s="81"/>
+      <c r="D5" s="82"/>
+      <c r="G5" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="74"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="82"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>38.880000000000003</v>
+        <v>43.98</v>
       </c>
       <c r="D6" s="16"/>
       <c r="G6" s="14"/>
@@ -1435,7 +1438,7 @@
       </c>
       <c r="C8" s="18">
         <f>C6*C7</f>
-        <v>3628.2982017600002</v>
+        <v>4104.2323794599997</v>
       </c>
       <c r="D8" s="16"/>
       <c r="G8" s="14"/>
@@ -1528,7 +1531,7 @@
       </c>
       <c r="C12" s="19">
         <f>C8-C11</f>
-        <v>3731.2982017600002</v>
+        <v>4207.2323794599997</v>
       </c>
       <c r="D12" s="17"/>
       <c r="G12" s="14"/>
@@ -1570,11 +1573,11 @@
       <c r="Q14" s="6"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="73"/>
-      <c r="D15" s="74"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="82"/>
       <c r="G15" s="14"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -1591,10 +1594,10 @@
       <c r="B16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="68" t="s">
+      <c r="C16" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="69"/>
+      <c r="D16" s="78"/>
       <c r="G16" s="14"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -1614,10 +1617,10 @@
       <c r="B17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="69"/>
+      <c r="D17" s="78"/>
       <c r="G17" s="14"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1637,10 +1640,10 @@
       <c r="B18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="69"/>
+      <c r="D18" s="78"/>
       <c r="G18" s="14"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1657,10 +1660,10 @@
       <c r="B19" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="70" t="s">
+      <c r="C19" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="71"/>
+      <c r="D19" s="86"/>
       <c r="G19" s="14"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1700,11 +1703,11 @@
       <c r="Q21" s="6"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="72" t="s">
+      <c r="B22" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="74"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="82"/>
       <c r="G22" s="14"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -1721,10 +1724,10 @@
       <c r="B23" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="68" t="s">
+      <c r="C23" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="69"/>
+      <c r="D23" s="78"/>
       <c r="G23" s="14"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1741,10 +1744,10 @@
       <c r="B24" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="68">
+      <c r="C24" s="77">
         <v>1879</v>
       </c>
-      <c r="D24" s="69"/>
+      <c r="D24" s="78"/>
       <c r="G24" s="14"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1761,11 +1764,11 @@
       <c r="B25" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="77">
+      <c r="C25" s="79">
         <f>'Financial Model'!U33</f>
         <v>2794</v>
       </c>
-      <c r="D25" s="69"/>
+      <c r="D25" s="78"/>
       <c r="G25" s="14"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -1780,8 +1783,8 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B26" s="12"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="69"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="78"/>
       <c r="G26" s="14"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -1798,11 +1801,11 @@
       <c r="B27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="77">
+      <c r="C27" s="79">
         <f>'Financial Model'!U33</f>
         <v>2794</v>
       </c>
-      <c r="D27" s="69"/>
+      <c r="D27" s="78"/>
       <c r="G27" s="14"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -1819,11 +1822,11 @@
       <c r="B28" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="77">
+      <c r="C28" s="79">
         <f>'Financial Model'!U42</f>
         <v>1685</v>
       </c>
-      <c r="D28" s="69"/>
+      <c r="D28" s="78"/>
       <c r="G28" s="14"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -1838,8 +1841,8 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B29" s="12"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="69"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="78"/>
       <c r="G29" s="14"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -1878,10 +1881,10 @@
       <c r="B31" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="75" t="s">
+      <c r="C31" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="76"/>
+      <c r="D31" s="84"/>
       <c r="G31" s="15"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
@@ -1895,83 +1898,81 @@
       <c r="Q31" s="8"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="73"/>
-      <c r="D34" s="74"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="82"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="66">
+      <c r="C35" s="75">
         <f>C6/'Financial Model'!U67</f>
-        <v>1.1142657256827251</v>
-      </c>
-      <c r="D35" s="67"/>
+        <v>1.2604271248849341</v>
+      </c>
+      <c r="D35" s="76"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="66">
+      <c r="C36" s="75">
         <f>C8/SUM('Financial Model'!R6:U6)</f>
-        <v>0.41447317817683349</v>
-      </c>
-      <c r="D36" s="67"/>
+        <v>0.4688408018574366</v>
+      </c>
+      <c r="D36" s="76"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="66">
+      <c r="C37" s="75">
         <f>C12/SUM('Financial Model'!R6:U6)</f>
-        <v>0.42623922798263653</v>
-      </c>
-      <c r="D37" s="67"/>
+        <v>0.48060685166323963</v>
+      </c>
+      <c r="D37" s="76"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="66">
+      <c r="C38" s="75">
         <f>C6/SUM('Financial Model'!R18:U18)</f>
-        <v>8.8454790838610293</v>
-      </c>
-      <c r="D38" s="67"/>
+        <v>10.005765692083539</v>
+      </c>
+      <c r="D38" s="76"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="66">
+      <c r="C39" s="75">
         <f>C12/SUM('Financial Model'!R17:U17)</f>
-        <v>8.8002316079245286</v>
-      </c>
-      <c r="D39" s="67"/>
+        <v>9.9227178760849046</v>
+      </c>
+      <c r="D39" s="76"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="68"/>
-      <c r="D40" s="69"/>
+      <c r="C40" s="77"/>
+      <c r="D40" s="78"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="13"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="71"/>
+      <c r="C41" s="85"/>
+      <c r="D41" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
     <mergeCell ref="G5:Q5"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C31:D31"/>
@@ -1984,11 +1985,13 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C31:D31" r:id="rId1" display="Link" xr:uid="{895B3114-FB4F-46F5-A7E6-2022E34FF531}"/>
@@ -2003,11 +2006,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9C1236-EF31-448C-82ED-0941EE456E01}">
   <dimension ref="A1:EE86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="Z4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AL20" sqref="AL20"/>
+      <selection pane="bottomRight" activeCell="AR21" sqref="AR21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4696,10 +4699,10 @@
       </c>
     </row>
     <row r="20" spans="2:135" x14ac:dyDescent="0.2">
-      <c r="AV20" s="79" t="s">
+      <c r="AV20" s="67" t="s">
         <v>136</v>
       </c>
-      <c r="AW20" s="80">
+      <c r="AW20" s="68">
         <v>0.01</v>
       </c>
     </row>
@@ -4755,11 +4758,11 @@
         <f>V6/R6-1</f>
         <v>-2.5352413498504922E-2</v>
       </c>
-      <c r="AD21" s="78" t="s">
+      <c r="AD21" s="66" t="s">
         <v>132</v>
       </c>
       <c r="AE21" s="28">
-        <f t="shared" ref="AE21:AH21" si="57">AE6/AD6-1</f>
+        <f t="shared" ref="AE21:AG21" si="57">AE6/AD6-1</f>
         <v>2.0174762271909508E-2</v>
       </c>
       <c r="AF21" s="28">
@@ -4814,7 +4817,7 @@
       <c r="AV21" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="AW21" s="81">
+      <c r="AW21" s="69">
         <v>0.08</v>
       </c>
     </row>
@@ -4872,10 +4875,10 @@
         <v>0.29043510189094923</v>
       </c>
       <c r="AI22" s="53"/>
-      <c r="AV22" s="82" t="s">
+      <c r="AV22" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="AW22" s="83">
+      <c r="AW22" s="71">
         <f>NPV(AW21,AI17:EE17)</f>
         <v>10630.831829573717</v>
       </c>
@@ -4934,10 +4937,10 @@
         <v>-8.186577820085672E-2</v>
       </c>
       <c r="AI23" s="53"/>
-      <c r="AV23" s="82" t="s">
+      <c r="AV23" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="AW23" s="83">
+      <c r="AW23" s="71">
         <f>Main!C11</f>
         <v>-103</v>
       </c>
@@ -5021,10 +5024,10 @@
         <v>132</v>
       </c>
       <c r="AI24" s="53"/>
-      <c r="AV24" s="84" t="s">
+      <c r="AV24" s="72" t="s">
         <v>140</v>
       </c>
-      <c r="AW24" s="83">
+      <c r="AW24" s="71">
         <f>AW22+AW23</f>
         <v>10527.831829573717</v>
       </c>
@@ -5033,7 +5036,7 @@
       <c r="AV25" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="AW25" s="86">
+      <c r="AW25" s="74">
         <f>AW24/Main!C7</f>
         <v>112.81379830777797</v>
       </c>
@@ -5106,15 +5109,15 @@
         <v>0.32</v>
       </c>
       <c r="AD26" s="29">
-        <f t="shared" ref="AD26:AE26" si="82">AD8/AD6</f>
+        <f t="shared" ref="AD26" si="82">AD8/AD6</f>
         <v>0.31560010280133644</v>
       </c>
       <c r="AE26" s="29">
-        <f t="shared" ref="AE26:AF26" si="83">AE8/AE6</f>
+        <f t="shared" ref="AE26" si="83">AE8/AE6</f>
         <v>0.31842801360372841</v>
       </c>
       <c r="AF26" s="29">
-        <f t="shared" ref="AF26:AG26" si="84">AF8/AF6</f>
+        <f t="shared" ref="AF26" si="84">AF8/AF6</f>
         <v>0.31767645221736412</v>
       </c>
       <c r="AG26" s="29">
@@ -5165,9 +5168,9 @@
       <c r="AV26" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="AW26" s="83">
+      <c r="AW26" s="71">
         <f>Main!C6</f>
-        <v>38.880000000000003</v>
+        <v>43.98</v>
       </c>
     </row>
     <row r="27" spans="2:135" x14ac:dyDescent="0.2">
@@ -5239,15 +5242,15 @@
         <v>7.4389805623123681E-2</v>
       </c>
       <c r="AD27" s="29">
-        <f t="shared" ref="AD27:AE27" si="95">AD12/AD6</f>
+        <f t="shared" ref="AD27" si="95">AD12/AD6</f>
         <v>7.3374453867900286E-2</v>
       </c>
       <c r="AE27" s="29">
-        <f t="shared" ref="AE27:AF27" si="96">AE12/AE6</f>
+        <f t="shared" ref="AE27" si="96">AE12/AE6</f>
         <v>8.8046353445018266E-2</v>
       </c>
       <c r="AF27" s="29">
-        <f t="shared" ref="AF27:AG27" si="97">AF12/AF6</f>
+        <f t="shared" ref="AF27" si="97">AF12/AF6</f>
         <v>8.1074328544659582E-2</v>
       </c>
       <c r="AG27" s="29">
@@ -5309,9 +5312,9 @@
       <c r="AV27" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="AW27" s="85">
+      <c r="AW27" s="73">
         <f>AW25/AW26-1</f>
-        <v>1.9015894626486101</v>
+        <v>1.5651159233237375</v>
       </c>
     </row>
     <row r="28" spans="2:135" x14ac:dyDescent="0.2">
@@ -5383,15 +5386,15 @@
         <v>4.9253875484846533E-2</v>
       </c>
       <c r="AD28" s="29">
-        <f t="shared" ref="AD28:AE28" si="109">AD17/AD6</f>
+        <f t="shared" ref="AD28" si="109">AD17/AD6</f>
         <v>3.6494474428167563E-2</v>
       </c>
       <c r="AE28" s="29">
-        <f t="shared" ref="AE28:AF28" si="110">AE17/AE6</f>
+        <f t="shared" ref="AE28" si="110">AE17/AE6</f>
         <v>6.8144602594785234E-2</v>
       </c>
       <c r="AF28" s="29">
-        <f t="shared" ref="AF28:AG28" si="111">AF17/AF6</f>
+        <f t="shared" ref="AF28" si="111">AF17/AF6</f>
         <v>6.1336664584634604E-2</v>
       </c>
       <c r="AG28" s="29">
@@ -5519,15 +5522,15 @@
         <v>0.33</v>
       </c>
       <c r="AD29" s="29">
-        <f t="shared" ref="AD29:AE29" si="123">AD16/AD15</f>
+        <f t="shared" ref="AD29" si="123">AD16/AD15</f>
         <v>0.50865051903114189</v>
       </c>
       <c r="AE29" s="29">
-        <f t="shared" ref="AE29:AF29" si="124">AE16/AE15</f>
+        <f t="shared" ref="AE29" si="124">AE16/AE15</f>
         <v>0.24123422159887797</v>
       </c>
       <c r="AF29" s="29">
-        <f t="shared" ref="AF29:AG29" si="125">AF16/AF15</f>
+        <f t="shared" ref="AF29" si="125">AF16/AF15</f>
         <v>0.26934523809523808</v>
       </c>
       <c r="AG29" s="29">

</xml_diff>